<commit_message>
A bunch of changes to accomodate new excel sheet formats. Still need to test compileUpdate.pl.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29AA8E3-A69E-1E40-96FE-138F01DE4C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EAE548-F636-F842-A7D3-8E3CFEAD2B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49020" yWindow="0" windowWidth="32420" windowHeight="23600" activeTab="4" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="12800" windowHeight="17300" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="489">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1018,9 +1018,6 @@
     <t>location_sampler_type</t>
   </si>
   <si>
-    <t>county_lab_code</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -1400,6 +1397,114 @@
   </si>
   <si>
     <t>Huntington, WV 25755</t>
+  </si>
+  <si>
+    <t>county_id</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>JJ</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>LL</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>OO</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>QQ</t>
+  </si>
+  <si>
+    <t>RR</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>UU</t>
+  </si>
+  <si>
+    <t>VV</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>YY</t>
+  </si>
+  <si>
+    <t>ZZ</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>CCC</t>
   </si>
 </sst>
 </file>
@@ -1967,7 +2072,7 @@
   <dimension ref="A1:S74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
@@ -1996,7 +2101,7 @@
         <v>200</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>232</v>
@@ -2008,7 +2113,7 @@
         <v>233</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G1" s="18" t="s">
         <v>234</v>
@@ -2017,7 +2122,7 @@
         <v>235</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>251</v>
@@ -2029,16 +2134,16 @@
         <v>325</v>
       </c>
       <c r="M1" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>353</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>354</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="P1" s="18" t="s">
         <v>355</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>356</v>
       </c>
       <c r="Q1" s="18" t="s">
         <v>236</v>
@@ -2055,7 +2160,7 @@
         <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>60</v>
@@ -2067,7 +2172,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>157</v>
@@ -2087,7 +2192,7 @@
         <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>103</v>
@@ -2096,10 +2201,10 @@
         <v>64</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G3" s="2">
         <v>-79.50179</v>
@@ -2118,7 +2223,7 @@
         <v>700</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M3" s="23">
         <v>24</v>
@@ -2130,7 +2235,7 @@
         <v>20</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>20</v>
@@ -2145,7 +2250,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>60</v>
@@ -2154,10 +2259,10 @@
         <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G4" s="2">
         <v>-81.015979999999999</v>
@@ -2175,7 +2280,7 @@
         <v>2391</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M4" s="23">
         <v>24</v>
@@ -2187,7 +2292,7 @@
         <v>20</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>20</v>
@@ -2202,7 +2307,7 @@
         <v>112</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C5" s="34" t="s">
         <v>190</v>
@@ -2211,10 +2316,10 @@
         <v>119</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G5" s="2">
         <v>-79.936940000000007</v>
@@ -2232,7 +2337,7 @@
         <v>1974</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M5" s="23">
         <v>24</v>
@@ -2240,7 +2345,7 @@
       <c r="N5" s="23"/>
       <c r="O5" s="23"/>
       <c r="P5" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>20</v>
@@ -2254,7 +2359,7 @@
         <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>190</v>
@@ -2263,10 +2368,10 @@
         <v>117</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G6" s="2">
         <v>-80.212010000000006</v>
@@ -2284,7 +2389,7 @@
         <v>400</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M6" s="23">
         <v>24</v>
@@ -2292,7 +2397,7 @@
       <c r="N6" s="23"/>
       <c r="O6" s="23"/>
       <c r="P6" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>20</v>
@@ -2307,7 +2412,7 @@
         <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C7" s="34" t="s">
         <v>190</v>
@@ -2316,10 +2421,10 @@
         <v>94</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G7" s="2">
         <v>-80.258989999999997</v>
@@ -2337,7 +2442,7 @@
         <v>6984</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M7" s="23">
         <v>24</v>
@@ -2345,7 +2450,7 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>20</v>
@@ -2360,7 +2465,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>60</v>
@@ -2372,7 +2477,7 @@
         <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G8" s="2">
         <v>-79.905010000000004</v>
@@ -2390,7 +2495,7 @@
         <v>579</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M8" s="24">
         <v>8</v>
@@ -2398,7 +2503,7 @@
       <c r="N8" s="24"/>
       <c r="O8" s="24"/>
       <c r="P8" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>20</v>
@@ -2413,7 +2518,7 @@
         <v>174</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>60</v>
@@ -2422,10 +2527,10 @@
         <v>156</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G9" s="2">
         <v>-82.285698770801503</v>
@@ -2434,7 +2539,7 @@
         <v>38.414946823509098</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>157</v>
@@ -2443,7 +2548,7 @@
         <v>4000</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M9" s="24">
         <v>8.3333329999999997E-2</v>
@@ -2472,7 +2577,7 @@
         <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>190</v>
@@ -2481,10 +2586,10 @@
         <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G10" s="2">
         <v>-80.567440000000005</v>
@@ -2502,7 +2607,7 @@
         <v>1340</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M10" s="23">
         <v>24</v>
@@ -2514,7 +2619,7 @@
         <v>30</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q10" s="2" t="s">
         <v>20</v>
@@ -2529,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>103</v>
@@ -2538,10 +2643,10 @@
         <v>68</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G11" s="2">
         <v>-81.677679999999995</v>
@@ -2559,7 +2664,7 @@
         <v>50000</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M11" s="23">
         <v>24</v>
@@ -2567,7 +2672,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>20</v>
@@ -2582,7 +2687,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>103</v>
@@ -2591,10 +2696,10 @@
         <v>69</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G12" s="2">
         <v>-77.855890000000002</v>
@@ -2612,7 +2717,7 @@
         <v>17000</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M12" s="23">
         <v>24</v>
@@ -2620,7 +2725,7 @@
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>20</v>
@@ -2635,7 +2740,7 @@
         <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>60</v>
@@ -2647,7 +2752,7 @@
         <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G13" s="2">
         <v>-79.867609999999999</v>
@@ -2665,7 +2770,7 @@
         <v>830</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M13" s="24">
         <v>8</v>
@@ -2673,7 +2778,7 @@
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
       <c r="P13" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>20</v>
@@ -2688,7 +2793,7 @@
         <v>101</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>103</v>
@@ -2697,10 +2802,10 @@
         <v>102</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G14" s="2">
         <v>-79.856999999999999</v>
@@ -2718,7 +2823,7 @@
         <v>2000</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M14" s="23">
         <v>24</v>
@@ -2730,7 +2835,7 @@
         <v>20</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>20</v>
@@ -2745,7 +2850,7 @@
         <v>93</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>103</v>
@@ -2754,10 +2859,10 @@
         <v>95</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G15" s="2">
         <v>-80.338570000000004</v>
@@ -2775,7 +2880,7 @@
         <v>26498</v>
       </c>
       <c r="L15" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M15" s="23">
         <v>24</v>
@@ -2783,7 +2888,7 @@
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>20</v>
@@ -2798,7 +2903,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>60</v>
@@ -2810,7 +2915,7 @@
         <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G16" s="2">
         <v>-79.945801900000006</v>
@@ -2828,7 +2933,7 @@
         <v>567</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M16" s="24">
         <v>48</v>
@@ -2840,7 +2945,7 @@
         <v>30</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>20</v>
@@ -2857,7 +2962,7 @@
         <v>188</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>60</v>
@@ -2869,7 +2974,7 @@
         <v>19</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -2894,7 +2999,7 @@
         <v>173</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>60</v>
@@ -2903,10 +3008,10 @@
         <v>68</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G18" s="2">
         <v>-81.679554234298493</v>
@@ -2915,7 +3020,7 @@
         <v>38.373735533484897</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>1</v>
@@ -2924,7 +3029,7 @@
         <v>49500</v>
       </c>
       <c r="L18" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M18" s="23">
         <v>24</v>
@@ -2932,7 +3037,7 @@
       <c r="N18" s="23"/>
       <c r="O18" s="23"/>
       <c r="P18" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>20</v>
@@ -2947,7 +3052,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>60</v>
@@ -2959,7 +3064,7 @@
         <v>19</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G19" s="2">
         <v>-79.953093199999998</v>
@@ -2977,7 +3082,7 @@
         <v>639</v>
       </c>
       <c r="L19" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M19" s="24">
         <v>48</v>
@@ -2989,7 +3094,7 @@
         <v>30</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q19" s="2" t="s">
         <v>20</v>
@@ -3006,7 +3111,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C20" s="33" t="s">
         <v>60</v>
@@ -3018,7 +3123,7 @@
         <v>19</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G20" s="2">
         <v>-80.000420899999995</v>
@@ -3036,7 +3141,7 @@
         <v>912</v>
       </c>
       <c r="L20" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M20" s="24">
         <v>48</v>
@@ -3048,7 +3153,7 @@
         <v>30</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>20</v>
@@ -3065,7 +3170,7 @@
         <v>181</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>60</v>
@@ -3074,10 +3179,10 @@
         <v>164</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G21" s="2">
         <v>-81.758709180509001</v>
@@ -3086,7 +3191,7 @@
         <v>38.368519014596998</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>1</v>
@@ -3095,7 +3200,7 @@
         <v>9000</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M21" s="23">
         <v>24</v>
@@ -3107,7 +3212,7 @@
         <v>20</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q21" s="2" t="s">
         <v>20</v>
@@ -3121,7 +3226,7 @@
         <v>113</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>103</v>
@@ -3130,10 +3235,10 @@
         <v>120</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G22" s="2">
         <v>-79.865430000000003</v>
@@ -3151,7 +3256,7 @@
         <v>13156</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M22" s="23">
         <v>24</v>
@@ -3163,7 +3268,7 @@
         <v>20</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>20</v>
@@ -3178,7 +3283,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>103</v>
@@ -3187,10 +3292,10 @@
         <v>138</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G23" s="2">
         <v>-79.972157499999994</v>
@@ -3208,7 +3313,7 @@
         <v>324</v>
       </c>
       <c r="L23" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M23" s="24">
         <v>48</v>
@@ -3220,7 +3325,7 @@
         <v>30</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>20</v>
@@ -3237,7 +3342,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C24" s="33" t="s">
         <v>60</v>
@@ -3249,7 +3354,7 @@
         <v>19</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G24" s="2">
         <v>-79.956234100000003</v>
@@ -3267,7 +3372,7 @@
         <v>324</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M24" s="24">
         <v>48</v>
@@ -3279,7 +3384,7 @@
         <v>30</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>20</v>
@@ -3296,7 +3401,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C25" s="33" t="s">
         <v>60</v>
@@ -3308,7 +3413,7 @@
         <v>19</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G25" s="2">
         <v>-79.956204600000007</v>
@@ -3326,7 +3431,7 @@
         <v>324</v>
       </c>
       <c r="L25" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M25" s="24">
         <v>48</v>
@@ -3338,7 +3443,7 @@
         <v>30</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q25" s="2" t="s">
         <v>20</v>
@@ -3355,7 +3460,7 @@
         <v>91</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>190</v>
@@ -3364,10 +3469,10 @@
         <v>97</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G26" s="2">
         <v>-80.124449999999996</v>
@@ -3385,7 +3490,7 @@
         <v>25525</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M26" s="23">
         <v>24</v>
@@ -3397,7 +3502,7 @@
         <v>30</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>20</v>
@@ -3412,7 +3517,7 @@
         <v>109</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>103</v>
@@ -3421,10 +3526,10 @@
         <v>116</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G27" s="2">
         <v>-80.24933</v>
@@ -3442,7 +3547,7 @@
         <v>610</v>
       </c>
       <c r="L27" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M27" s="23">
         <v>24</v>
@@ -3454,7 +3559,7 @@
         <v>20</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>20</v>
@@ -3469,7 +3574,7 @@
         <v>111</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C28" s="33" t="s">
         <v>60</v>
@@ -3478,10 +3583,10 @@
         <v>118</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G28" s="2">
         <v>-80.598290000000006</v>
@@ -3499,7 +3604,7 @@
         <v>6468</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M28" s="23">
         <v>24</v>
@@ -3511,7 +3616,7 @@
         <v>20</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>20</v>
@@ -3526,7 +3631,7 @@
         <v>99</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>103</v>
@@ -3535,10 +3640,10 @@
         <v>98</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G29" s="2">
         <v>-80.018370000000004</v>
@@ -3556,7 +3661,7 @@
         <v>6071</v>
       </c>
       <c r="L29" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M29" s="23">
         <v>24</v>
@@ -3564,7 +3669,7 @@
       <c r="N29" s="23"/>
       <c r="O29" s="23"/>
       <c r="P29" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>20</v>
@@ -3579,7 +3684,7 @@
         <v>244</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>60</v>
@@ -3591,7 +3696,7 @@
         <v>124</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G30" s="2">
         <v>-79.515240000000006</v>
@@ -3626,7 +3731,7 @@
         <v>201</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>103</v>
@@ -3638,7 +3743,7 @@
         <v>19</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G31" s="2">
         <v>-79.956762600000005</v>
@@ -3656,7 +3761,7 @@
         <v>874</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M31" s="24">
         <v>48</v>
@@ -3668,7 +3773,7 @@
         <v>30</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q31" s="2" t="s">
         <v>20</v>
@@ -3685,7 +3790,7 @@
         <v>175</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C32" s="33" t="s">
         <v>60</v>
@@ -3694,10 +3799,10 @@
         <v>160</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G32" s="2">
         <v>-82.006959612418996</v>
@@ -3706,7 +3811,7 @@
         <v>38.446524084559897</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>161</v>
@@ -3715,7 +3820,7 @@
         <v>28759</v>
       </c>
       <c r="L32" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M32" s="23">
         <v>72</v>
@@ -3727,7 +3832,7 @@
         <v>20</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q32" s="2" t="s">
         <v>20</v>
@@ -3742,7 +3847,7 @@
         <v>172</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>60</v>
@@ -3751,10 +3856,10 @@
         <v>155</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G33" s="2">
         <v>-82.528864034905197</v>
@@ -3763,7 +3868,7 @@
         <v>38.400744931017101</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>191</v>
@@ -3772,7 +3877,7 @@
         <v>56000</v>
       </c>
       <c r="L33" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M33" s="23">
         <v>24</v>
@@ -3784,7 +3889,7 @@
         <v>20</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q33" s="2" t="s">
         <v>20</v>
@@ -3799,7 +3904,7 @@
         <v>108</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>103</v>
@@ -3808,10 +3913,10 @@
         <v>115</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G34" s="2">
         <v>-79.978949999999998</v>
@@ -3829,7 +3934,7 @@
         <v>2101</v>
       </c>
       <c r="L34" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M34" s="23">
         <v>24</v>
@@ -3841,7 +3946,7 @@
         <v>20</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>20</v>
@@ -3856,7 +3961,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>103</v>
@@ -3865,10 +3970,10 @@
         <v>71</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G35" s="2">
         <v>-78.975080000000005</v>
@@ -3886,7 +3991,7 @@
         <v>8168</v>
       </c>
       <c r="L35" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M35" s="23">
         <v>24</v>
@@ -3898,7 +4003,7 @@
         <v>20</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q35" s="2" t="s">
         <v>20</v>
@@ -3913,7 +4018,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>60</v>
@@ -3925,7 +4030,7 @@
         <v>19</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G36" s="2">
         <v>-79.955122099999997</v>
@@ -3943,7 +4048,7 @@
         <v>324</v>
       </c>
       <c r="L36" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M36" s="24">
         <v>48</v>
@@ -3955,7 +4060,7 @@
         <v>30</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q36" s="2" t="s">
         <v>20</v>
@@ -3972,7 +4077,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>60</v>
@@ -3984,7 +4089,7 @@
         <v>19</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G37" s="2">
         <v>-79.955245399999995</v>
@@ -4002,7 +4107,7 @@
         <v>324</v>
       </c>
       <c r="L37" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M37" s="24">
         <v>48</v>
@@ -4014,7 +4119,7 @@
         <v>30</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q37" s="2" t="s">
         <v>20</v>
@@ -4031,7 +4136,7 @@
         <v>152</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>103</v>
@@ -4040,10 +4145,10 @@
         <v>154</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G38" s="2">
         <v>-81.847288800000001</v>
@@ -4061,7 +4166,7 @@
         <v>4555</v>
       </c>
       <c r="L38" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M38" s="23">
         <v>24</v>
@@ -4073,7 +4178,7 @@
         <v>20</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>20</v>
@@ -4088,7 +4193,7 @@
         <v>104</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>103</v>
@@ -4097,10 +4202,10 @@
         <v>105</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G39" s="2">
         <v>-80.323710000000005</v>
@@ -4118,7 +4223,7 @@
         <v>1091</v>
       </c>
       <c r="L39" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M39" s="23">
         <v>24</v>
@@ -4130,7 +4235,7 @@
         <v>20</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q39" s="2" t="s">
         <v>20</v>
@@ -4145,7 +4250,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>60</v>
@@ -4157,7 +4262,7 @@
         <v>34</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G40" s="2">
         <v>-79.957359999999994</v>
@@ -4175,7 +4280,7 @@
         <v>1851</v>
       </c>
       <c r="L40" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M40" s="24">
         <v>8</v>
@@ -4183,7 +4288,7 @@
       <c r="N40" s="24"/>
       <c r="O40" s="24"/>
       <c r="P40" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q40" s="2" t="s">
         <v>20</v>
@@ -4198,7 +4303,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>103</v>
@@ -4207,10 +4312,10 @@
         <v>73</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G41" s="2">
         <v>-80.754930000000002</v>
@@ -4228,7 +4333,7 @@
         <v>12000</v>
       </c>
       <c r="L41" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M41" s="23">
         <v>24</v>
@@ -4236,7 +4341,7 @@
       <c r="N41" s="23"/>
       <c r="O41" s="23"/>
       <c r="P41" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q41" s="2" t="s">
         <v>20</v>
@@ -4251,7 +4356,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>60</v>
@@ -4263,7 +4368,7 @@
         <v>34</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G42" s="2">
         <v>-79.943309999999997</v>
@@ -4281,7 +4386,7 @@
         <v>726</v>
       </c>
       <c r="L42" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M42" s="24">
         <v>8</v>
@@ -4289,7 +4394,7 @@
       <c r="N42" s="24"/>
       <c r="O42" s="24"/>
       <c r="P42" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>20</v>
@@ -4303,7 +4408,7 @@
         <v>31</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>103</v>
@@ -4315,7 +4420,7 @@
         <v>19</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G43" s="2">
         <v>-79.965769100000003</v>
@@ -4333,7 +4438,7 @@
         <v>324</v>
       </c>
       <c r="L43" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M43" s="24">
         <v>48</v>
@@ -4345,7 +4450,7 @@
         <v>30</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q43" s="2" t="s">
         <v>20</v>
@@ -4362,7 +4467,7 @@
         <v>165</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>60</v>
@@ -4371,10 +4476,10 @@
         <v>166</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G44" s="2">
         <v>-82.451303840583293</v>
@@ -4383,7 +4488,7 @@
         <v>38.343336164586603</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>167</v>
@@ -4392,7 +4497,7 @@
         <v>1600</v>
       </c>
       <c r="L44" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M44" s="23">
         <v>24</v>
@@ -4404,7 +4509,7 @@
         <v>20</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>20</v>
@@ -4421,7 +4526,7 @@
         <v>36</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C45" s="33" t="s">
         <v>60</v>
@@ -4433,7 +4538,7 @@
         <v>34</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G45" s="2">
         <v>-79.956739999999996</v>
@@ -4451,7 +4556,7 @@
         <v>688</v>
       </c>
       <c r="L45" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M45" s="24">
         <v>8</v>
@@ -4459,7 +4564,7 @@
       <c r="N45" s="24"/>
       <c r="O45" s="24"/>
       <c r="P45" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q45" s="2" t="s">
         <v>20</v>
@@ -4470,10 +4575,10 @@
     </row>
     <row r="46" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>103</v>
@@ -4485,7 +4590,7 @@
         <v>19</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G46" s="2">
         <v>-79.953202899999994</v>
@@ -4503,7 +4608,7 @@
         <v>324</v>
       </c>
       <c r="L46" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M46" s="24">
         <v>48</v>
@@ -4515,7 +4620,7 @@
         <v>30</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q46" s="2" t="s">
         <v>20</v>
@@ -4532,7 +4637,7 @@
         <v>23</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>103</v>
@@ -4544,7 +4649,7 @@
         <v>19</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G47" s="2">
         <v>-79.962211800000006</v>
@@ -4562,7 +4667,7 @@
         <v>862</v>
       </c>
       <c r="L47" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M47" s="24">
         <v>48</v>
@@ -4574,7 +4679,7 @@
         <v>30</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q47" s="2" t="s">
         <v>20</v>
@@ -4591,7 +4696,7 @@
         <v>49</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>103</v>
@@ -4600,10 +4705,10 @@
         <v>76</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G48" s="2">
         <v>-81.557389999999998</v>
@@ -4621,7 +4726,7 @@
         <v>48050</v>
       </c>
       <c r="L48" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M48" s="23">
         <v>24</v>
@@ -4629,7 +4734,7 @@
       <c r="N48" s="23"/>
       <c r="O48" s="23"/>
       <c r="P48" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q48" s="2" t="s">
         <v>20</v>
@@ -4643,7 +4748,7 @@
         <v>169</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>60</v>
@@ -4652,10 +4757,10 @@
         <v>170</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G49" s="2">
         <v>-82.287563960345196</v>
@@ -4664,7 +4769,7 @@
         <v>38.572623654172197</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J49" s="2" t="s">
         <v>157</v>
@@ -4673,7 +4778,7 @@
         <v>1000</v>
       </c>
       <c r="L49" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M49" s="23">
         <v>24</v>
@@ -4685,7 +4790,7 @@
         <v>20</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q49" s="2" t="s">
         <v>20</v>
@@ -4702,7 +4807,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>60</v>
@@ -4711,10 +4816,10 @@
         <v>77</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G50" s="2">
         <v>-79.127250000000004</v>
@@ -4732,7 +4837,7 @@
         <v>2700</v>
       </c>
       <c r="L50" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M50" s="23">
         <v>24</v>
@@ -4740,7 +4845,7 @@
       <c r="N50" s="23"/>
       <c r="O50" s="23"/>
       <c r="P50" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>20</v>
@@ -4754,7 +4859,7 @@
         <v>197</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>103</v>
@@ -4763,10 +4868,10 @@
         <v>198</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G51" s="2">
         <v>-82.135114799999997</v>
@@ -4784,7 +4889,7 @@
         <v>5515</v>
       </c>
       <c r="L51" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M51" s="23">
         <v>24</v>
@@ -4796,7 +4901,7 @@
         <v>20</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>20</v>
@@ -4810,7 +4915,7 @@
         <v>59</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C52" s="34" t="s">
         <v>190</v>
@@ -4822,7 +4927,7 @@
         <v>19</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G52" s="2">
         <v>-78.98272</v>
@@ -4840,7 +4945,7 @@
         <v>1193</v>
       </c>
       <c r="L52" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M52" s="24">
         <v>48</v>
@@ -4852,7 +4957,7 @@
         <v>30</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q52" s="2" t="s">
         <v>20</v>
@@ -4866,7 +4971,7 @@
         <v>16</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>103</v>
@@ -4875,10 +4980,10 @@
         <v>78</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G53" s="2">
         <v>-81.079930000000004</v>
@@ -4896,7 +5001,7 @@
         <v>36000</v>
       </c>
       <c r="L53" s="24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M53" s="23">
         <v>24</v>
@@ -4908,7 +5013,7 @@
         <v>20</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q53" s="2" t="s">
         <v>20</v>
@@ -4922,7 +5027,7 @@
         <v>180</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C54" s="33" t="s">
         <v>60</v>
@@ -4931,10 +5036,10 @@
         <v>163</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G54" s="2">
         <v>-82.298209254857795</v>
@@ -4943,7 +5048,7 @@
         <v>38.419661908139098</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>157</v>
@@ -4952,7 +5057,7 @@
         <v>7000</v>
       </c>
       <c r="L54" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M54" s="23">
         <v>24</v>
@@ -4964,7 +5069,7 @@
         <v>20</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q54" s="2" t="s">
         <v>20</v>
@@ -4978,7 +5083,7 @@
         <v>106</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>103</v>
@@ -4987,10 +5092,10 @@
         <v>107</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G55" s="2">
         <v>-80.545150000000007</v>
@@ -5008,7 +5113,7 @@
         <v>1853</v>
       </c>
       <c r="L55" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M55" s="23">
         <v>24</v>
@@ -5020,7 +5125,7 @@
         <v>20</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q55" s="2" t="s">
         <v>20</v>
@@ -5034,7 +5139,7 @@
         <v>193</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>103</v>
@@ -5046,7 +5151,7 @@
         <v>19</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G56" s="2">
         <v>-79.956140000000005</v>
@@ -5064,7 +5169,7 @@
         <v>474</v>
       </c>
       <c r="L56" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M56" s="24">
         <v>48</v>
@@ -5076,7 +5181,7 @@
         <v>30</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q56" s="2" t="s">
         <v>20</v>
@@ -5093,7 +5198,7 @@
         <v>125</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C57" s="34" t="s">
         <v>190</v>
@@ -5102,10 +5207,10 @@
         <v>128</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -5119,7 +5224,7 @@
         <v>1800</v>
       </c>
       <c r="L57" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M57" s="23">
         <v>24</v>
@@ -5127,7 +5232,7 @@
       <c r="N57" s="23"/>
       <c r="O57" s="23"/>
       <c r="P57" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q57" s="2" t="s">
         <v>20</v>
@@ -5140,7 +5245,7 @@
         <v>178</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>60</v>
@@ -5149,10 +5254,10 @@
         <v>179</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G58" s="2">
         <v>-82.105144999999993</v>
@@ -5161,7 +5266,7 @@
         <v>38.425437000000002</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J58" s="2" t="s">
         <v>157</v>
@@ -5170,7 +5275,7 @@
         <v>7200</v>
       </c>
       <c r="L58" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M58" s="23">
         <v>24</v>
@@ -5182,7 +5287,7 @@
         <v>20</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q58" s="2" t="s">
         <v>20</v>
@@ -5199,7 +5304,7 @@
         <v>176</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C59" s="33" t="s">
         <v>60</v>
@@ -5208,10 +5313,10 @@
         <v>177</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G59" s="2">
         <v>-82.244877751268803</v>
@@ -5220,7 +5325,7 @@
         <v>38.372162360135</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="J59" s="2" t="s">
         <v>157</v>
@@ -5229,7 +5334,7 @@
         <v>4050</v>
       </c>
       <c r="L59" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M59" s="23">
         <v>24</v>
@@ -5241,7 +5346,7 @@
         <v>20</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q59" s="2" t="s">
         <v>20</v>
@@ -5258,7 +5363,7 @@
         <v>10</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>103</v>
@@ -5267,10 +5372,10 @@
         <v>137</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G60" s="2">
         <v>-79.992055399999998</v>
@@ -5288,7 +5393,7 @@
         <v>48328</v>
       </c>
       <c r="L60" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M60" s="23">
         <v>24</v>
@@ -5296,7 +5401,7 @@
       <c r="N60" s="23"/>
       <c r="O60" s="23"/>
       <c r="P60" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q60" s="2" t="s">
         <v>20</v>
@@ -5311,7 +5416,7 @@
         <v>51</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C61" s="33" t="s">
         <v>60</v>
@@ -5320,10 +5425,10 @@
         <v>79</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G61" s="2">
         <v>-81.205110000000005</v>
@@ -5341,7 +5446,7 @@
         <v>2892</v>
       </c>
       <c r="L61" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M61" s="23">
         <v>24</v>
@@ -5353,7 +5458,7 @@
         <v>20</v>
       </c>
       <c r="P61" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q61" s="2" t="s">
         <v>20</v>
@@ -5368,7 +5473,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C62" s="33" t="s">
         <v>60</v>
@@ -5380,7 +5485,7 @@
         <v>34</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G62" s="2">
         <v>-79.978250000000003</v>
@@ -5398,7 +5503,7 @@
         <v>515</v>
       </c>
       <c r="L62" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M62" s="24">
         <v>8</v>
@@ -5406,7 +5511,7 @@
       <c r="N62" s="24"/>
       <c r="O62" s="24"/>
       <c r="P62" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q62" s="2" t="s">
         <v>20</v>
@@ -5421,7 +5526,7 @@
         <v>24</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>103</v>
@@ -5433,7 +5538,7 @@
         <v>19</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G63" s="2">
         <v>-79.966336100000007</v>
@@ -5451,7 +5556,7 @@
         <v>904</v>
       </c>
       <c r="L63" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M63" s="24">
         <v>48</v>
@@ -5463,7 +5568,7 @@
         <v>30</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q63" s="2" t="s">
         <v>20</v>
@@ -5480,7 +5585,7 @@
         <v>184</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C64" s="33" t="s">
         <v>60</v>
@@ -5492,7 +5597,7 @@
         <v>19</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -5517,7 +5622,7 @@
         <v>186</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C65" s="33" t="s">
         <v>60</v>
@@ -5529,7 +5634,7 @@
         <v>19</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -5554,7 +5659,7 @@
         <v>37</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C66" s="33" t="s">
         <v>60</v>
@@ -5566,7 +5671,7 @@
         <v>34</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G66" s="2">
         <v>-79.926150000000007</v>
@@ -5584,7 +5689,7 @@
         <v>1310</v>
       </c>
       <c r="L66" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M66" s="24">
         <v>8</v>
@@ -5592,7 +5697,7 @@
       <c r="N66" s="24"/>
       <c r="O66" s="24"/>
       <c r="P66" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q66" s="2" t="s">
         <v>20</v>
@@ -5607,7 +5712,7 @@
         <v>32</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>103</v>
@@ -5619,7 +5724,7 @@
         <v>19</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G67" s="2">
         <v>-79.956755900000005</v>
@@ -5637,7 +5742,7 @@
         <v>324</v>
       </c>
       <c r="L67" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M67" s="24">
         <v>48</v>
@@ -5649,7 +5754,7 @@
         <v>30</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q67" s="2" t="s">
         <v>20</v>
@@ -5666,7 +5771,7 @@
         <v>14</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C68" s="34" t="s">
         <v>190</v>
@@ -5675,10 +5780,10 @@
         <v>82</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G68" s="2">
         <v>-78.226619999999997</v>
@@ -5696,7 +5801,7 @@
         <v>3255</v>
       </c>
       <c r="L68" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M68" s="23">
         <v>24</v>
@@ -5704,7 +5809,7 @@
       <c r="N68" s="23"/>
       <c r="O68" s="23"/>
       <c r="P68" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q68" s="2" t="s">
         <v>20</v>
@@ -5719,7 +5824,7 @@
         <v>126</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C69" s="34" t="s">
         <v>190</v>
@@ -5728,10 +5833,10 @@
         <v>127</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -5745,7 +5850,7 @@
         <v>20411</v>
       </c>
       <c r="L69" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M69" s="23">
         <v>24</v>
@@ -5753,7 +5858,7 @@
       <c r="N69" s="23"/>
       <c r="O69" s="23"/>
       <c r="P69" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q69" s="2" t="s">
         <v>20</v>
@@ -5766,7 +5871,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>103</v>
@@ -5775,10 +5880,10 @@
         <v>83</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G70" s="2">
         <v>-80.459909999999994</v>
@@ -5796,7 +5901,7 @@
         <v>10364</v>
       </c>
       <c r="L70" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M70" s="23">
         <v>24</v>
@@ -5808,7 +5913,7 @@
         <v>20</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q70" s="2" t="s">
         <v>20</v>
@@ -5823,7 +5928,7 @@
         <v>33</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C71" s="33" t="s">
         <v>60</v>
@@ -5835,7 +5940,7 @@
         <v>19</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G71" s="2">
         <v>-79.925397000000004</v>
@@ -5853,7 +5958,7 @@
         <v>324</v>
       </c>
       <c r="L71" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M71" s="24">
         <v>48</v>
@@ -5865,7 +5970,7 @@
         <v>30</v>
       </c>
       <c r="P71" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q71" s="2" t="s">
         <v>20</v>
@@ -5882,7 +5987,7 @@
         <v>52</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>103</v>
@@ -5891,10 +5996,10 @@
         <v>84</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G72" s="2">
         <v>-80.778989999999993</v>
@@ -5912,7 +6017,7 @@
         <v>564</v>
       </c>
       <c r="L72" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M72" s="23">
         <v>24</v>
@@ -5924,7 +6029,7 @@
         <v>20</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q72" s="2" t="s">
         <v>20</v>
@@ -5939,7 +6044,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>103</v>
@@ -5948,10 +6053,10 @@
         <v>85</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G73" s="2">
         <v>-80.72757</v>
@@ -5969,7 +6074,7 @@
         <v>50000</v>
       </c>
       <c r="L73" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="M73" s="23">
         <v>24</v>
@@ -5977,7 +6082,7 @@
       <c r="N73" s="23"/>
       <c r="O73" s="23"/>
       <c r="P73" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q73" s="2" t="s">
         <v>20</v>
@@ -5992,7 +6097,7 @@
         <v>90</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C74" s="34" t="s">
         <v>190</v>
@@ -6001,10 +6106,10 @@
         <v>96</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G74" s="2">
         <v>-80.260360000000006</v>
@@ -6022,7 +6127,7 @@
         <v>2742</v>
       </c>
       <c r="L74" s="24" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="M74" s="23">
         <v>24</v>
@@ -6034,7 +6139,7 @@
         <v>30</v>
       </c>
       <c r="P74" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="Q74" s="2" t="s">
         <v>20</v>
@@ -6056,7 +6161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
@@ -6211,10 +6316,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
@@ -6329,10 +6434,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14" t="s">
@@ -6348,10 +6453,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14" t="s">
@@ -6485,13 +6590,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>370</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>371</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>191</v>
@@ -6677,10 +6782,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14" t="s">
@@ -6696,10 +6801,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14" t="s">
@@ -6753,10 +6858,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14" t="s">
@@ -6772,10 +6877,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14" t="s">
@@ -6947,10 +7052,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>157</v>
@@ -6975,767 +7080,837 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A1:D56"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="19" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="26">
+      <c r="B2" s="26">
         <v>54061</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="27">
+      <c r="D2" s="27">
         <v>105612</v>
       </c>
-      <c r="D2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="26">
+      <c r="B3" s="26">
         <v>54039</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="C3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="29">
+      <c r="D3" s="29">
         <v>183279</v>
       </c>
-      <c r="D3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="26">
+      <c r="B4" s="26">
         <v>54069</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27">
+      <c r="D4" s="27">
         <v>41411</v>
       </c>
-      <c r="D4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="26">
+      <c r="B5" s="26">
         <v>54037</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="C5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27">
+      <c r="D5" s="27">
         <v>57146</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="28"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
+      <c r="B6" s="26">
         <v>54055</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="C6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="27">
+      <c r="D6" s="27">
         <v>58758</v>
       </c>
-      <c r="D6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="26">
+      <c r="B7" s="26">
         <v>54041</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="C7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="27">
+      <c r="D7" s="27">
         <v>16166</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="E7" s="30"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="26">
+      <c r="B8" s="26">
         <v>54057</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="C8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="27">
+      <c r="D8" s="27">
         <v>26868</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="30"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="E8" s="30"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="26">
+      <c r="B9" s="26">
         <v>54051</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="C9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="27">
+      <c r="D9" s="27">
         <v>30531</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="E9" s="30"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="26">
+      <c r="B10" s="26">
         <v>54065</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="C10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="27">
+      <c r="D10" s="27">
         <v>17884</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="E10" s="30"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="26">
+      <c r="B11" s="26">
         <v>54077</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="C11" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="27">
+      <c r="D11" s="27">
         <v>33432</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="30"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="E11" s="30"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="26">
+      <c r="B12" s="26">
         <v>54107</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="C12" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="27">
+      <c r="D12" s="27">
         <v>83518</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="30"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="E12" s="30"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="26">
+      <c r="B13" s="26">
         <v>54017</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="C13" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="27">
+      <c r="D13" s="27">
         <v>8448</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="E13" s="30"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="26">
+      <c r="B14" s="26">
         <v>54049</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="C14" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="27">
+      <c r="D14" s="27">
         <v>56072</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="30"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>339</v>
       </c>
-      <c r="E14" s="30"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="26">
+      <c r="B15" s="26">
         <v>54033</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="C15" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="27">
+      <c r="D15" s="27">
         <v>67256</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="E15" s="30"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="26">
+      <c r="B16" s="26">
         <v>54091</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="C16" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="27">
+      <c r="D16" s="27">
         <v>16695</v>
       </c>
-      <c r="D16" s="4" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="26">
+      <c r="B17" s="26">
         <v>54073</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="C17" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="27">
+      <c r="D17" s="27">
         <v>7482</v>
       </c>
-      <c r="D17" s="4" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="26">
+      <c r="B18" s="26">
         <v>54005</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="C18" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="C18" s="27">
+      <c r="D18" s="27">
         <v>21809</v>
       </c>
-      <c r="D18" s="4" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="26">
+      <c r="B19" s="26">
         <v>54083</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="C19" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="27">
+      <c r="D19" s="27">
         <v>28695</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="26">
+      <c r="B20" s="26">
         <v>54009</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="C20" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="27">
+      <c r="D20" s="27">
         <v>21939</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="E20" s="31"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="26">
+      <c r="B21" s="26">
         <v>54053</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="C21" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="C21" s="27">
+      <c r="D21" s="27">
         <v>26700</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>346</v>
-      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="26">
+      <c r="A22" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B22" s="26">
         <v>54001</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="C22" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="27">
+      <c r="D22" s="27">
         <v>16633</v>
       </c>
-      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="26">
+      <c r="A23" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B23" s="26">
         <v>54003</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="C23" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="C23" s="27">
+      <c r="D23" s="27">
         <v>126069</v>
       </c>
-      <c r="D23" s="4"/>
       <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="26">
+      <c r="A24" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="B24" s="26">
         <v>54007</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="C24" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="C24" s="27">
+      <c r="D24" s="27">
         <v>12247</v>
       </c>
-      <c r="D24" s="4"/>
       <c r="E24" s="30"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="26">
+      <c r="A25" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="B25" s="26">
         <v>54011</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="C25" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="C25" s="29">
+      <c r="D25" s="29">
         <v>96319</v>
       </c>
-      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="26">
+      <c r="A26" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="B26" s="26">
         <v>54013</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="C26" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="C26" s="27">
+      <c r="D26" s="27">
         <v>6176</v>
       </c>
-      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="26">
+      <c r="A27" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B27" s="26">
         <v>54015</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="C27" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="C27" s="27">
+      <c r="D27" s="27">
         <v>7892</v>
       </c>
-      <c r="D27" s="4"/>
       <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="26">
+      <c r="A28" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B28" s="26">
         <v>54019</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="C28" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="C28" s="27">
+      <c r="D28" s="27">
         <v>39927</v>
       </c>
-      <c r="D28" s="4"/>
       <c r="E28" s="31"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="26">
+      <c r="A29" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B29" s="26">
         <v>54021</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="C29" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="27">
+      <c r="D29" s="27">
         <v>7377</v>
       </c>
-      <c r="D29" s="4"/>
       <c r="E29" s="31"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="26">
+      <c r="A30" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B30" s="26">
         <v>54023</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="C30" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="27">
+      <c r="D30" s="27">
         <v>11616</v>
       </c>
-      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="26">
+      <c r="A31" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B31" s="26">
         <v>54025</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="C31" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="27">
+      <c r="D31" s="27">
         <v>32608</v>
       </c>
-      <c r="D31" s="4"/>
       <c r="E31" s="31"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="26">
+      <c r="A32" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B32" s="26">
         <v>54027</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="C32" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="27">
+      <c r="D32" s="27">
         <v>23302</v>
       </c>
-      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="26">
+      <c r="A33" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B33" s="26">
         <v>54029</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="C33" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="C33" s="27">
+      <c r="D33" s="27">
         <v>28656</v>
       </c>
-      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="26">
+      <c r="A34" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B34" s="26">
         <v>54031</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="C34" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="C34" s="27">
+      <c r="D34" s="27">
         <v>14160</v>
       </c>
-      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="26">
+      <c r="A35" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="B35" s="26">
         <v>54035</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="C35" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="C35" s="27">
+      <c r="D35" s="27">
         <v>27738</v>
       </c>
-      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="26">
+      <c r="A36" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="B36" s="26">
         <v>54043</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="C36" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="C36" s="27">
+      <c r="D36" s="27">
         <v>20126</v>
       </c>
-      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="26">
+      <c r="A37" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B37" s="26">
         <v>54045</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="C37" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="C37" s="27">
+      <c r="D37" s="27">
         <v>31909</v>
       </c>
-      <c r="D37" s="4"/>
       <c r="E37" s="28"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="26">
+      <c r="A38" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B38" s="26">
         <v>54047</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="C38" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="C38" s="27">
+      <c r="D38" s="27">
         <v>18363</v>
       </c>
-      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="26">
+      <c r="A39" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B39" s="26">
         <v>54059</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="C39" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="C39" s="27">
+      <c r="D39" s="27">
         <v>23005</v>
       </c>
-      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="26">
+      <c r="A40" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="B40" s="26">
         <v>54063</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="C40" s="26" t="s">
         <v>217</v>
       </c>
-      <c r="C40" s="27">
+      <c r="D40" s="27">
         <v>12332</v>
       </c>
-      <c r="D40" s="4"/>
       <c r="E40" s="28"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="26">
+      <c r="A41" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="B41" s="26">
         <v>54067</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="C41" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="C41" s="27">
+      <c r="D41" s="27">
         <v>24300</v>
       </c>
-      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="26">
+      <c r="A42" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B42" s="26">
         <v>54071</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="C42" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="C42" s="27">
+      <c r="D42" s="27">
         <v>6142</v>
       </c>
-      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="26">
+      <c r="A43" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B43" s="26">
         <v>54075</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="C43" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="C43" s="27">
+      <c r="D43" s="27">
         <v>7841</v>
       </c>
-      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="26">
+      <c r="A44" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B44" s="26">
         <v>54079</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="C44" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="C44" s="29">
+      <c r="D44" s="29">
         <v>55486</v>
       </c>
-      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="26">
+      <c r="A45" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B45" s="26">
         <v>54081</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="C45" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C45" s="27">
+      <c r="D45" s="27">
         <v>73771</v>
       </c>
-      <c r="D45" s="4"/>
       <c r="E45" s="28"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="26">
+      <c r="A46" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="B46" s="26">
         <v>54085</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="C46" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C46" s="27">
+      <c r="D46" s="27">
         <v>8383</v>
       </c>
-      <c r="D46" s="4"/>
       <c r="E46" s="28"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="26">
+      <c r="A47" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="B47" s="26">
         <v>54087</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="C47" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="C47" s="27">
+      <c r="D47" s="27">
         <v>13898</v>
       </c>
-      <c r="D47" s="4"/>
       <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="26">
+      <c r="A48" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B48" s="26">
         <v>54089</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="C48" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C48" s="27">
+      <c r="D48" s="27">
         <v>11908</v>
       </c>
-      <c r="D48" s="4"/>
       <c r="E48" s="28"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="26">
+      <c r="A49" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B49" s="26">
         <v>54093</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="C49" s="26" t="s">
         <v>225</v>
       </c>
-      <c r="C49" s="27">
+      <c r="D49" s="27">
         <v>6672</v>
       </c>
-      <c r="D49" s="4"/>
       <c r="E49" s="28"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="26">
+      <c r="A50" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B50" s="26">
         <v>54095</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="C50" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="27">
+      <c r="D50" s="27">
         <v>8811</v>
       </c>
-      <c r="D50" s="4"/>
       <c r="E50" s="28"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="26">
+      <c r="A51" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="B51" s="26">
         <v>54097</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="C51" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="C51" s="27">
+      <c r="D51" s="27">
         <v>23791</v>
       </c>
-      <c r="D51" s="4"/>
       <c r="E51" s="28"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="26">
+      <c r="A52" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B52" s="26">
         <v>54099</v>
       </c>
-      <c r="B52" s="26" t="s">
+      <c r="C52" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C52" s="29">
+      <c r="D52" s="29">
         <v>42481</v>
       </c>
-      <c r="D52" s="4"/>
       <c r="E52" s="28"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="26">
+      <c r="A53" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B53" s="26">
         <v>54101</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="C53" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="C53" s="27">
+      <c r="D53" s="27">
         <v>8249</v>
       </c>
-      <c r="D53" s="4"/>
       <c r="E53" s="28"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="26">
+      <c r="A54" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="B54" s="26">
         <v>54103</v>
       </c>
-      <c r="B54" s="26" t="s">
+      <c r="C54" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="C54" s="27">
+      <c r="D54" s="27">
         <v>14170</v>
       </c>
-      <c r="D54" s="4"/>
       <c r="E54" s="28"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="26">
+      <c r="A55" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B55" s="26">
         <v>54105</v>
       </c>
-      <c r="B55" s="26" t="s">
+      <c r="C55" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="C55" s="27">
+      <c r="D55" s="27">
         <v>5063</v>
       </c>
-      <c r="D55" s="4"/>
       <c r="E55" s="28"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="26">
+      <c r="A56" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="B56" s="26">
         <v>54109</v>
       </c>
-      <c r="B56" s="26" t="s">
+      <c r="C56" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="C56" s="27">
+      <c r="D56" s="27">
         <v>21051</v>
       </c>
-      <c r="D56" s="4"/>
       <c r="E56" s="28"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D57" s="4"/>
+      <c r="A57" s="4"/>
       <c r="E57" s="28"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -7751,13 +7926,12 @@
       <c r="E61" s="28"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D62" s="10"/>
+      <c r="A62" s="10"/>
       <c r="E62" s="31"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D56">
-    <sortCondition ref="D2:D56"/>
-    <sortCondition ref="B2:B56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D56">
+    <sortCondition ref="C2:C56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7767,9 +7941,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="157" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7784,279 +7958,279 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>384</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="35" t="s">
         <v>385</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>386</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="E1" s="35" t="s">
         <v>387</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>388</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>390</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>390</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D2" s="36" t="s">
+      <c r="E2" s="36" t="s">
         <v>391</v>
       </c>
-      <c r="E2" s="36" t="s">
-        <v>392</v>
-      </c>
       <c r="F2" s="36" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
+        <v>392</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>393</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="C3" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="F3" s="36" t="s">
         <v>394</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>391</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
+        <v>395</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>396</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="C4" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>397</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>391</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="F4" s="36" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
+        <v>421</v>
+      </c>
+      <c r="B5" s="36" t="s">
         <v>422</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>423</v>
-      </c>
       <c r="C5" s="36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="36" t="s">
         <v>437</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>401</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>438</v>
-      </c>
       <c r="D6" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>391</v>
       </c>
-      <c r="E6" s="36" t="s">
-        <v>392</v>
-      </c>
       <c r="F6" s="36" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D7" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="E7" s="36" t="s">
         <v>391</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>392</v>
-      </c>
       <c r="F7" s="36" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="F8" s="36" t="s">
         <v>403</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>403</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>391</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B9" s="36" t="s">
+        <v>404</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D9" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="E9" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="F9" s="36" t="s">
         <v>406</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D10" s="36" t="s">
+        <v>405</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="F10" s="36" t="s">
         <v>406</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B12" s="36" t="s">
+        <v>409</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D12" s="36" t="s">
         <v>410</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D12" s="36" t="s">
+      <c r="E12" s="36" t="s">
+        <v>391</v>
+      </c>
+      <c r="F12" s="36" t="s">
         <v>411</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>392</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
+        <v>427</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>428</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>429</v>
-      </c>
       <c r="C13" s="36" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D13" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="E13" s="36" t="s">
         <v>391</v>
       </c>
-      <c r="E13" s="36" t="s">
-        <v>392</v>
-      </c>
       <c r="F13" s="36" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
+        <v>433</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>434</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="C14" s="36" t="s">
+        <v>439</v>
+      </c>
+      <c r="D14" s="36" t="s">
         <v>435</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>440</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>436</v>
-      </c>
       <c r="E14" s="36" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F14" s="36" t="s">
         <v>324</v>
@@ -8064,59 +8238,59 @@
     </row>
     <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B15" s="36" t="s">
+        <v>412</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D15" s="36" t="s">
         <v>413</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D15" s="36" t="s">
+      <c r="E15" s="36" t="s">
         <v>414</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="F15" s="36" t="s">
         <v>415</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B16" s="36" t="s">
+        <v>416</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="E16" s="36" t="s">
         <v>417</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>391</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>418</v>
-      </c>
       <c r="F16" s="36" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B17" s="36" t="s">
+        <v>418</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>437</v>
+      </c>
+      <c r="D17" s="36" t="s">
         <v>419</v>
       </c>
-      <c r="C17" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="D17" s="36" t="s">
+      <c r="E17" s="36" t="s">
         <v>420</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>421</v>
       </c>
       <c r="F17" s="36" t="s">
         <v>324</v>
@@ -8131,7 +8305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6D3376-E2B9-1B45-B67A-A3F205C129CA}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -8146,53 +8320,53 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
+        <v>440</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>441</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="37" t="s">
         <v>442</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>443</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="37" t="s">
         <v>444</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C2" t="s">
         <v>446</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>447</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>448</v>
-      </c>
-      <c r="E2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C3" t="s">
         <v>450</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>451</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>452</v>
-      </c>
-      <c r="E3" t="s">
-        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major upgrade to a full working patchr workflow.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EAE548-F636-F842-A7D3-8E3CFEAD2B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BF8BDE-1FF6-504D-92D2-25298841E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="12800" windowHeight="17300" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="502">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1505,6 +1505,45 @@
   </si>
   <si>
     <t>CCC</t>
+  </si>
+  <si>
+    <t>StadiumSW-01</t>
+  </si>
+  <si>
+    <t>WVU Stadium SW</t>
+  </si>
+  <si>
+    <t>StadiumNW-01</t>
+  </si>
+  <si>
+    <t>WVU Stadium NW</t>
+  </si>
+  <si>
+    <t>StadiumNE-01</t>
+  </si>
+  <si>
+    <t>WVU Stadium NE</t>
+  </si>
+  <si>
+    <t>StadiumSE-01</t>
+  </si>
+  <si>
+    <t>WVU Stadium SE</t>
+  </si>
+  <si>
+    <t>Coliseum-01</t>
+  </si>
+  <si>
+    <t>WVU Coliseum</t>
+  </si>
+  <si>
+    <t>WhiteOakWWTP-01</t>
+  </si>
+  <si>
+    <t>White Oak</t>
+  </si>
+  <si>
+    <t>White Oak WWTP</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1553,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1632,8 +1671,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1652,6 +1703,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1666,7 +1723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1749,6 +1806,23 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2069,18 +2143,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:S74"/>
+  <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C74" sqref="C74"/>
+      <selection pane="bottomRight" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="22.1640625" customWidth="1"/>
@@ -3717,7 +3792,9 @@
       <c r="M30" s="23"/>
       <c r="N30" s="23"/>
       <c r="O30" s="23"/>
-      <c r="P30" s="2"/>
+      <c r="P30" s="2" t="s">
+        <v>356</v>
+      </c>
       <c r="Q30" s="2" t="s">
         <v>20</v>
       </c>
@@ -6148,6 +6225,308 @@
         <v>26591</v>
       </c>
       <c r="S74" s="2"/>
+    </row>
+    <row r="75" spans="1:19" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="38" t="s">
+        <v>489</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C75" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D75" s="38" t="s">
+        <v>490</v>
+      </c>
+      <c r="E75" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G75" s="40"/>
+      <c r="I75" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J75" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L75" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="M75" s="41">
+        <v>12</v>
+      </c>
+      <c r="N75" s="23">
+        <v>25</v>
+      </c>
+      <c r="O75" s="23">
+        <v>30</v>
+      </c>
+      <c r="P75" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q75" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R75" s="39">
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="38" t="s">
+        <v>491</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C76" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D76" s="38" t="s">
+        <v>492</v>
+      </c>
+      <c r="E76" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G76" s="40"/>
+      <c r="I76" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J76" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L76" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="M76" s="41">
+        <v>12</v>
+      </c>
+      <c r="N76" s="23">
+        <v>25</v>
+      </c>
+      <c r="O76" s="23">
+        <v>30</v>
+      </c>
+      <c r="P76" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q76" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R76" s="39">
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="38" t="s">
+        <v>493</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C77" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D77" s="38" t="s">
+        <v>494</v>
+      </c>
+      <c r="E77" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G77" s="40"/>
+      <c r="I77" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J77" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L77" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="M77" s="41">
+        <v>12</v>
+      </c>
+      <c r="N77" s="23">
+        <v>25</v>
+      </c>
+      <c r="O77" s="23">
+        <v>30</v>
+      </c>
+      <c r="P77" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q77" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R77" s="39">
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" s="38" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="38" t="s">
+        <v>495</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C78" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D78" s="38" t="s">
+        <v>496</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G78" s="40"/>
+      <c r="I78" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J78" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L78" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="M78" s="41">
+        <v>12</v>
+      </c>
+      <c r="N78" s="23">
+        <v>25</v>
+      </c>
+      <c r="O78" s="23">
+        <v>30</v>
+      </c>
+      <c r="P78" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q78" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R78" s="39">
+        <v>26505</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A79" s="38" t="s">
+        <v>497</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C79" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D79" s="38" t="s">
+        <v>498</v>
+      </c>
+      <c r="E79" s="38" t="s">
+        <v>350</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G79">
+        <v>-79.985057699999999</v>
+      </c>
+      <c r="H79">
+        <v>39.648165400000003</v>
+      </c>
+      <c r="I79" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J79" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="L79" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="M79" s="8">
+        <v>8</v>
+      </c>
+      <c r="N79" s="23">
+        <v>25</v>
+      </c>
+      <c r="O79" s="23">
+        <v>30</v>
+      </c>
+      <c r="P79" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q79" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R79" s="39">
+        <v>26505</v>
+      </c>
+      <c r="S79" s="38"/>
+    </row>
+    <row r="80" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="G80" s="14">
+        <v>-81.1824412</v>
+      </c>
+      <c r="H80" s="14">
+        <v>37.946477700000003</v>
+      </c>
+      <c r="I80" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="J80" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="K80" s="44">
+        <v>2626</v>
+      </c>
+      <c r="L80" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="M80" s="15">
+        <v>24</v>
+      </c>
+      <c r="N80" s="15">
+        <v>25</v>
+      </c>
+      <c r="O80" s="15">
+        <v>30</v>
+      </c>
+      <c r="P80" s="46" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q80" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R80" s="26">
+        <v>25917</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S74">
@@ -6159,11 +6538,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6818,7 +7197,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>275</v>
       </c>
@@ -6837,7 +7216,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>276</v>
       </c>
@@ -6856,7 +7235,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>379</v>
       </c>
@@ -6875,7 +7254,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>380</v>
       </c>
@@ -6894,7 +7273,7 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>240</v>
       </c>
@@ -6917,7 +7296,7 @@
         <v>48328</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>277</v>
       </c>
@@ -6936,7 +7315,7 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>278</v>
       </c>
@@ -6955,7 +7334,7 @@
         <v>3255</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>279</v>
       </c>
@@ -6974,7 +7353,7 @@
         <v>20411</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>280</v>
       </c>
@@ -6993,7 +7372,7 @@
         <v>10364</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>281</v>
       </c>
@@ -7012,7 +7391,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>282</v>
       </c>
@@ -7031,7 +7410,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>283</v>
       </c>
@@ -7050,7 +7429,7 @@
         <v>2742</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>363</v>
       </c>
@@ -7066,6 +7445,34 @@
       <c r="G45" s="8">
         <v>1000</v>
       </c>
+    </row>
+    <row r="46" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="42" t="s">
+        <v>499</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" t="s">
+        <v>206</v>
+      </c>
+      <c r="E46" s="43">
+        <v>54001022001</v>
+      </c>
+      <c r="F46" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="G46" s="44">
+        <v>2626</v>
+      </c>
+      <c r="H46" s="44"/>
+      <c r="I46" s="45"/>
+      <c r="J46"/>
+      <c r="K46" s="1"/>
+      <c r="L46"/>
+      <c r="M46" s="2"/>
+      <c r="U46"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G47">
@@ -7080,7 +7487,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7941,7 +8348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
@@ -8305,8 +8712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6D3376-E2B9-1B45-B67A-A3F205C129CA}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Some file export code added to reportboard.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FC1544-6710-A847-B533-0319A57D06AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A810B81-0CFA-ED4F-99A1-E18B7BC08F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="760" windowWidth="25880" windowHeight="16820" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="31180" yWindow="9800" windowWidth="25880" windowHeight="16820" activeTab="2" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="606">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1853,6 +1853,9 @@
   </si>
   <si>
     <t>WV0020168</t>
+  </si>
+  <si>
+    <t>M04</t>
   </si>
 </sst>
 </file>
@@ -2446,11 +2449,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2944,7 +2947,7 @@
         <v>109</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>573</v>
+        <v>605</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>360</v>
@@ -7042,8 +7045,8 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8293,8 +8296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7DED6B-84CB-6D46-B3EB-C814548CEBA4}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Data update for last week of Jan 2024.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A810B81-0CFA-ED4F-99A1-E18B7BC08F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42B4C12-A117-6449-AE96-AD16BD61F039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31180" yWindow="9800" windowWidth="25880" windowHeight="16820" activeTab="2" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="50440" yWindow="5140" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="county" sheetId="2" r:id="rId3"/>
     <sheet name="target" sheetId="4" r:id="rId4"/>
     <sheet name="lab" sheetId="5" r:id="rId5"/>
+    <sheet name="loci" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="634">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1303,24 +1304,9 @@
     <t>Bacteria</t>
   </si>
   <si>
-    <t>Human Norovirus GII</t>
-  </si>
-  <si>
     <t>huNovGII</t>
   </si>
   <si>
-    <t>Mpox Virus Clade I</t>
-  </si>
-  <si>
-    <t>Mpox Virus Clade II</t>
-  </si>
-  <si>
-    <t>Escherichia coli, Shiga toxin-producing</t>
-  </si>
-  <si>
-    <t>Human Immunodeficiency Virus 1</t>
-  </si>
-  <si>
     <t>Enterovirus</t>
   </si>
   <si>
@@ -1330,36 +1316,12 @@
     <t>Rv</t>
   </si>
   <si>
-    <t>Pepper Mild Mottle Virus</t>
-  </si>
-  <si>
-    <t>Respiratory Syncitial Virus, Bovine</t>
-  </si>
-  <si>
-    <t>Cross-assembly phage</t>
-  </si>
-  <si>
-    <t>Human RNAse P</t>
-  </si>
-  <si>
-    <t>RP</t>
-  </si>
-  <si>
-    <t>Control</t>
-  </si>
-  <si>
-    <t>Respiratory Syncitial Virus, Human</t>
-  </si>
-  <si>
     <t>Viral</t>
   </si>
   <si>
     <t>Bacterial</t>
   </si>
   <si>
-    <t>Eukaryotic</t>
-  </si>
-  <si>
     <t>lab_id</t>
   </si>
   <si>
@@ -1856,6 +1818,129 @@
   </si>
   <si>
     <t>M04</t>
+  </si>
+  <si>
+    <t>WhiteOakWWTP</t>
+  </si>
+  <si>
+    <t>crAssphage</t>
+  </si>
+  <si>
+    <t>Enterococcus</t>
+  </si>
+  <si>
+    <t>Escherichia coli, Shiga toxin-producing (STEC)</t>
+  </si>
+  <si>
+    <t>Human Immunodeficiency Virus 1 (HIV-1)</t>
+  </si>
+  <si>
+    <t>Human Immunodeficiency Virus 2 (HIV-2)</t>
+  </si>
+  <si>
+    <t>Legionella</t>
+  </si>
+  <si>
+    <t>Pepper Mild Mottle Virus (PMMoV)</t>
+  </si>
+  <si>
+    <t>Respiratory Syncitial Virus, Bovine (BRSV)</t>
+  </si>
+  <si>
+    <t>Respiratory Syncitial Virus, Human (RSV)</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica serovar Enteritidis</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica serovar Javiana</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica serovar Newport</t>
+  </si>
+  <si>
+    <t>Salmonella enterica subsp. enterica serovar Typhimurium</t>
+  </si>
+  <si>
+    <t>HIV-2</t>
+  </si>
+  <si>
+    <t>Mpox Virus I (MPXV I)</t>
+  </si>
+  <si>
+    <t>Mpox Virus II (MPXV II)</t>
+  </si>
+  <si>
+    <t>Ec</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Lg</t>
+  </si>
+  <si>
+    <t>Salmonella Enteritidis</t>
+  </si>
+  <si>
+    <t>Salmonella Newport</t>
+  </si>
+  <si>
+    <t>Salmonella Typhimurium</t>
+  </si>
+  <si>
+    <t>Salmonella Javiana</t>
+  </si>
+  <si>
+    <t>Legionairre's Disease</t>
+  </si>
+  <si>
+    <t>16S</t>
+  </si>
+  <si>
+    <t>23S</t>
+  </si>
+  <si>
+    <t>C3b</t>
+  </si>
+  <si>
+    <t>N1:SARS</t>
+  </si>
+  <si>
+    <t>N2:SARS</t>
+  </si>
+  <si>
+    <t>NEP/NS1</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>RNase P</t>
+  </si>
+  <si>
+    <t>S:E484K</t>
+  </si>
+  <si>
+    <t>S:E484K WT</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70 WT</t>
+  </si>
+  <si>
+    <t>S:N501Y</t>
+  </si>
+  <si>
+    <t>S:N501Y WT</t>
+  </si>
+  <si>
+    <t>TNFR</t>
+  </si>
+  <si>
+    <t>locus_id</t>
   </si>
 </sst>
 </file>
@@ -1865,7 +1950,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1995,6 +2080,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2029,7 +2130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2127,6 +2228,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2151,9 +2255,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2191,7 +2295,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2297,7 +2401,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2439,7 +2543,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2449,11 +2553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD15"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2480,7 +2584,7 @@
         <v>200</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>358</v>
@@ -2542,7 +2646,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>360</v>
@@ -2602,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>570</v>
+        <v>557</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>360</v>
@@ -2658,7 +2762,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>360</v>
@@ -2714,7 +2818,7 @@
         <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>360</v>
@@ -2773,7 +2877,7 @@
         <v>93</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>571</v>
+        <v>558</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>360</v>
@@ -2826,10 +2930,10 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>360</v>
@@ -2838,7 +2942,7 @@
         <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>350</v>
@@ -2887,7 +2991,7 @@
         <v>113</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>572</v>
+        <v>559</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>360</v>
@@ -2947,7 +3051,7 @@
         <v>109</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>360</v>
@@ -3007,7 +3111,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>360</v>
@@ -3063,7 +3167,7 @@
         <v>108</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>576</v>
+        <v>563</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>360</v>
@@ -3123,7 +3227,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>360</v>
@@ -3183,7 +3287,7 @@
         <v>152</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>360</v>
@@ -3243,7 +3347,7 @@
         <v>104</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>360</v>
@@ -3303,7 +3407,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>360</v>
@@ -3359,7 +3463,7 @@
         <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>360</v>
@@ -3415,7 +3519,7 @@
         <v>197</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>360</v>
@@ -3475,7 +3579,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>360</v>
@@ -3535,7 +3639,7 @@
         <v>106</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>360</v>
@@ -3595,7 +3699,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>360</v>
@@ -3651,7 +3755,7 @@
         <v>8</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>360</v>
@@ -3710,7 +3814,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>360</v>
@@ -3770,7 +3874,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>360</v>
@@ -3822,10 +3926,10 @@
     </row>
     <row r="24" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>360</v>
@@ -3834,7 +3938,7 @@
         <v>103</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>349</v>
@@ -3849,7 +3953,7 @@
         <v>37.946477700000003</v>
       </c>
       <c r="J24" s="12" t="s">
-        <v>499</v>
+        <v>593</v>
       </c>
       <c r="K24" s="12" t="s">
         <v>206</v>
@@ -4623,7 +4727,7 @@
         <v>18</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>569</v>
+        <v>556</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>360</v>
@@ -4683,7 +4787,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>360</v>
@@ -4739,7 +4843,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>360</v>
@@ -4795,7 +4899,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>360</v>
@@ -4857,7 +4961,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>360</v>
@@ -4919,7 +5023,7 @@
         <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>360</v>
@@ -4981,7 +5085,7 @@
         <v>22</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>360</v>
@@ -5041,7 +5145,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>360</v>
@@ -5101,7 +5205,7 @@
         <v>28</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>360</v>
@@ -5161,7 +5265,7 @@
         <v>111</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>360</v>
@@ -5272,7 +5376,7 @@
         <v>201</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>360</v>
@@ -5334,7 +5438,7 @@
         <v>29</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>360</v>
@@ -5394,7 +5498,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>360</v>
@@ -5454,7 +5558,7 @@
         <v>38</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>360</v>
@@ -5509,7 +5613,7 @@
         <v>39</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>360</v>
@@ -5564,7 +5668,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>360</v>
@@ -5624,7 +5728,7 @@
         <v>36</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>360</v>
@@ -5680,7 +5784,7 @@
         <v>348</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>360</v>
@@ -5740,7 +5844,7 @@
         <v>23</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>360</v>
@@ -5856,7 +5960,7 @@
         <v>193</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>360</v>
@@ -5915,10 +6019,10 @@
     </row>
     <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>360</v>
@@ -5927,7 +6031,7 @@
         <v>60</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>350</v>
@@ -5969,10 +6073,10 @@
     </row>
     <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>360</v>
@@ -5981,7 +6085,7 @@
         <v>60</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>350</v>
@@ -6023,10 +6127,10 @@
     </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>360</v>
@@ -6035,7 +6139,7 @@
         <v>60</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>350</v>
@@ -6077,10 +6181,10 @@
     </row>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>360</v>
@@ -6089,7 +6193,7 @@
         <v>60</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>350</v>
@@ -6134,7 +6238,7 @@
         <v>51</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>360</v>
@@ -6194,7 +6298,7 @@
         <v>58</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>360</v>
@@ -6250,7 +6354,7 @@
         <v>24</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>360</v>
@@ -6312,7 +6416,7 @@
         <v>37</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>360</v>
@@ -6368,7 +6472,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>360</v>
@@ -6428,7 +6532,7 @@
         <v>33</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>360</v>
@@ -6766,7 +6870,7 @@
         <v>59</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>360</v>
@@ -6874,7 +6978,7 @@
         <v>14</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>360</v>
@@ -7046,7 +7150,7 @@
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7065,7 +7169,7 @@
         <v>239</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>238</v>
@@ -7077,7 +7181,7 @@
         <v>247</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>502</v>
+        <v>489</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>249</v>
@@ -7094,7 +7198,7 @@
         <v>284</v>
       </c>
       <c r="B2" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>64</v>
@@ -7106,7 +7210,7 @@
         <v>63</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>503</v>
+        <v>490</v>
       </c>
       <c r="G2" s="31">
         <v>54003906001</v>
@@ -7124,7 +7228,7 @@
         <v>253</v>
       </c>
       <c r="B3" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>286</v>
@@ -7136,7 +7240,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>504</v>
+        <v>491</v>
       </c>
       <c r="G3" s="17">
         <v>54002701001</v>
@@ -7161,7 +7265,7 @@
         <v>157</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="G4" s="31">
         <v>54000601001</v>
@@ -7188,7 +7292,7 @@
         <v>123</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="G5" s="31">
         <v>54000101001</v>
@@ -7215,7 +7319,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="G6" s="31">
         <v>54003031001</v>
@@ -7242,7 +7346,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="G7" s="31">
         <v>54001702001</v>
@@ -7267,7 +7371,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="G8" s="31">
         <v>54002510001</v>
@@ -7284,7 +7388,7 @@
         <v>366</v>
       </c>
       <c r="B9" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>371</v>
@@ -7294,7 +7398,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="G9" s="31">
         <v>54002003001</v>
@@ -7311,7 +7415,7 @@
         <v>258</v>
       </c>
       <c r="B10" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>291</v>
@@ -7321,7 +7425,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="G10" s="31">
         <v>54002003001</v>
@@ -7338,7 +7442,7 @@
         <v>259</v>
       </c>
       <c r="B11" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>292</v>
@@ -7348,7 +7452,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>506</v>
+        <v>493</v>
       </c>
       <c r="G11" s="31">
         <v>54001901001</v>
@@ -7365,7 +7469,7 @@
         <v>260</v>
       </c>
       <c r="B12" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>315</v>
@@ -7377,7 +7481,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>507</v>
+        <v>494</v>
       </c>
       <c r="G12" s="31">
         <v>54003045001</v>
@@ -7394,7 +7498,7 @@
         <v>261</v>
       </c>
       <c r="B13" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>293</v>
@@ -7404,7 +7508,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="G13" s="31">
         <v>54001703001</v>
@@ -7421,7 +7525,7 @@
         <v>367</v>
       </c>
       <c r="B14" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>372</v>
@@ -7431,7 +7535,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="G14" s="31">
         <v>54002007001</v>
@@ -7448,7 +7552,7 @@
         <v>262</v>
       </c>
       <c r="B15" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>294</v>
@@ -7458,7 +7562,7 @@
         <v>121</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="G15" s="31">
         <v>54004202001</v>
@@ -7483,7 +7587,7 @@
         <v>89</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="G16" s="31">
         <v>54002405001</v>
@@ -7500,7 +7604,7 @@
         <v>264</v>
       </c>
       <c r="B17" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>296</v>
@@ -7510,7 +7614,7 @@
         <v>89</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="G17" s="31">
         <v>54002408001</v>
@@ -7527,7 +7631,7 @@
         <v>265</v>
       </c>
       <c r="B18" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>297</v>
@@ -7537,7 +7641,7 @@
         <v>122</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="G18" s="17">
         <v>54000504001</v>
@@ -7554,7 +7658,7 @@
         <v>266</v>
       </c>
       <c r="B19" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>298</v>
@@ -7564,7 +7668,7 @@
         <v>100</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="G19" s="31">
         <v>54004602001</v>
@@ -7604,7 +7708,7 @@
         <v>362</v>
       </c>
       <c r="B21" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>369</v>
@@ -7616,7 +7720,7 @@
         <v>191</v>
       </c>
       <c r="F21" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="G21" s="31">
         <v>54000603001</v>
@@ -7633,7 +7737,7 @@
         <v>267</v>
       </c>
       <c r="B22" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>300</v>
@@ -7643,7 +7747,7 @@
         <v>121</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="G22" s="31">
         <v>54004215001</v>
@@ -7660,7 +7764,7 @@
         <v>252</v>
       </c>
       <c r="B23" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>301</v>
@@ -7670,7 +7774,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="G23" s="31">
         <v>54002803001</v>
@@ -7687,7 +7791,7 @@
         <v>268</v>
       </c>
       <c r="B24" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>302</v>
@@ -7697,7 +7801,7 @@
         <v>153</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="G24" s="31">
         <v>54000316001</v>
@@ -7714,7 +7818,7 @@
         <v>269</v>
       </c>
       <c r="B25" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>303</v>
@@ -7724,7 +7828,7 @@
         <v>89</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="G25" s="31">
         <v>54002415001</v>
@@ -7741,7 +7845,7 @@
         <v>270</v>
       </c>
       <c r="B26" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>304</v>
@@ -7751,7 +7855,7 @@
         <v>5</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="G26" s="31">
         <v>54002509001</v>
@@ -7768,7 +7872,7 @@
         <v>271</v>
       </c>
       <c r="B27" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>305</v>
@@ -7778,7 +7882,7 @@
         <v>54</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="G27" s="31">
         <v>54005405001</v>
@@ -7795,7 +7899,7 @@
         <v>364</v>
       </c>
       <c r="B28" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>374</v>
@@ -7805,7 +7909,7 @@
         <v>157</v>
       </c>
       <c r="F28" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="17">
@@ -7870,7 +7974,7 @@
         <v>55</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="G31" s="17">
         <v>54001205001</v>
@@ -7887,7 +7991,7 @@
         <v>273</v>
       </c>
       <c r="B32" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>316</v>
@@ -7897,7 +8001,7 @@
         <v>199</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="G32" s="17">
         <v>54002606001</v>
@@ -7914,7 +8018,7 @@
         <v>274</v>
       </c>
       <c r="B33" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>307</v>
@@ -7924,7 +8028,7 @@
         <v>17</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="G33" s="17">
         <v>54002716001</v>
@@ -7941,7 +8045,7 @@
         <v>275</v>
       </c>
       <c r="B34" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>308</v>
@@ -7951,7 +8055,7 @@
         <v>88</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="G34" s="31">
         <v>54001710001</v>
@@ -7968,7 +8072,7 @@
         <v>379</v>
       </c>
       <c r="B35" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>381</v>
@@ -7978,7 +8082,7 @@
         <v>157</v>
       </c>
       <c r="F35" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="17">
@@ -7993,7 +8097,7 @@
         <v>380</v>
       </c>
       <c r="B36" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>382</v>
@@ -8003,7 +8107,7 @@
         <v>157</v>
       </c>
       <c r="F36" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="17">
@@ -8026,7 +8130,7 @@
         <v>129</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="G37" s="31">
         <v>54004804001</v>
@@ -8043,7 +8147,7 @@
         <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>285</v>
@@ -8055,7 +8159,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="G38" s="31">
         <v>54003011001</v>
@@ -8072,7 +8176,7 @@
         <v>277</v>
       </c>
       <c r="B39" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>317</v>
@@ -8082,7 +8186,7 @@
         <v>56</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="G39" s="17">
         <v>54003703001</v>
@@ -8099,7 +8203,7 @@
         <v>278</v>
       </c>
       <c r="B40" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>310</v>
@@ -8109,7 +8213,7 @@
         <v>15</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="G40" s="31">
         <v>54003203001</v>
@@ -8134,7 +8238,7 @@
         <v>122</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="G41" s="31">
         <v>54000509001</v>
@@ -8151,7 +8255,7 @@
         <v>280</v>
       </c>
       <c r="B42" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>312</v>
@@ -8161,7 +8265,7 @@
         <v>9</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="G42" s="17">
         <v>54002102001</v>
@@ -8178,7 +8282,7 @@
         <v>281</v>
       </c>
       <c r="B43" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="C43" s="17" t="s">
         <v>318</v>
@@ -8188,7 +8292,7 @@
         <v>57</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="G43" s="31">
         <v>54000901001</v>
@@ -8205,7 +8309,7 @@
         <v>282</v>
       </c>
       <c r="B44" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>313</v>
@@ -8215,7 +8319,7 @@
         <v>3</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="G44" s="31">
         <v>54003508001</v>
@@ -8229,20 +8333,20 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>499</v>
+        <v>593</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
         <v>206</v>
       </c>
       <c r="F45" s="31" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="G45" s="31">
         <v>54001022001</v>
@@ -8296,8 +8400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7DED6B-84CB-6D46-B3EB-C814548CEBA4}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8313,10 +8417,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>248</v>
@@ -8685,7 +8789,7 @@
         <v>123</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="C22" s="17">
         <v>54001</v>
@@ -8702,7 +8806,7 @@
         <v>202</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="C23" s="17">
         <v>54003</v>
@@ -8720,7 +8824,7 @@
         <v>203</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="C24" s="17">
         <v>54007</v>
@@ -8738,7 +8842,7 @@
         <v>157</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="C25" s="17">
         <v>54011</v>
@@ -8755,7 +8859,7 @@
         <v>204</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="C26" s="17">
         <v>54013</v>
@@ -8772,7 +8876,7 @@
         <v>205</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="C27" s="17">
         <v>54015</v>
@@ -8790,7 +8894,7 @@
         <v>206</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="C28" s="17">
         <v>54019</v>
@@ -8808,7 +8912,7 @@
         <v>207</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="C29" s="17">
         <v>54021</v>
@@ -8826,7 +8930,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="C30" s="17">
         <v>54023</v>
@@ -8843,7 +8947,7 @@
         <v>208</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="C31" s="17">
         <v>54025</v>
@@ -8861,7 +8965,7 @@
         <v>209</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="C32" s="17">
         <v>54027</v>
@@ -8878,7 +8982,7 @@
         <v>210</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="C33" s="17">
         <v>54029</v>
@@ -8895,7 +8999,7 @@
         <v>211</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="C34" s="17">
         <v>54031</v>
@@ -8912,7 +9016,7 @@
         <v>212</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="C35" s="17">
         <v>54035</v>
@@ -8929,7 +9033,7 @@
         <v>213</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="C36" s="17">
         <v>54043</v>
@@ -8946,7 +9050,7 @@
         <v>214</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="C37" s="17">
         <v>54045</v>
@@ -8964,7 +9068,7 @@
         <v>215</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="C38" s="17">
         <v>54047</v>
@@ -8981,7 +9085,7 @@
         <v>216</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="C39" s="17">
         <v>54059</v>
@@ -8998,7 +9102,7 @@
         <v>217</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="C40" s="17">
         <v>54063</v>
@@ -9016,7 +9120,7 @@
         <v>218</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="C41" s="17">
         <v>54067</v>
@@ -9033,7 +9137,7 @@
         <v>219</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="C42" s="17">
         <v>54071</v>
@@ -9050,7 +9154,7 @@
         <v>220</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="C43" s="17">
         <v>54075</v>
@@ -9067,7 +9171,7 @@
         <v>161</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="C44" s="17">
         <v>54079</v>
@@ -9084,7 +9188,7 @@
         <v>221</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="C45" s="17">
         <v>54081</v>
@@ -9102,7 +9206,7 @@
         <v>222</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="C46" s="17">
         <v>54085</v>
@@ -9120,7 +9224,7 @@
         <v>223</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="C47" s="17">
         <v>54087</v>
@@ -9138,7 +9242,7 @@
         <v>224</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="C48" s="17">
         <v>54089</v>
@@ -9156,7 +9260,7 @@
         <v>225</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="C49" s="17">
         <v>54093</v>
@@ -9174,7 +9278,7 @@
         <v>129</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="C50" s="17">
         <v>54095</v>
@@ -9192,7 +9296,7 @@
         <v>226</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="C51" s="17">
         <v>54097</v>
@@ -9210,7 +9314,7 @@
         <v>167</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="C52" s="17">
         <v>54099</v>
@@ -9228,7 +9332,7 @@
         <v>227</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="C53" s="17">
         <v>54101</v>
@@ -9246,7 +9350,7 @@
         <v>228</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="C54" s="17">
         <v>54103</v>
@@ -9264,7 +9368,7 @@
         <v>229</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="C55" s="17">
         <v>54105</v>
@@ -9282,7 +9386,7 @@
         <v>230</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="C56" s="17">
         <v>54109</v>
@@ -9325,24 +9429,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>383</v>
       </c>
@@ -9362,15 +9466,15 @@
         <v>388</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>389</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>389</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>390</v>
@@ -9382,55 +9486,50 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>392</v>
+    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="43" t="s">
+        <v>594</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>393</v>
+        <v>418</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>390</v>
+        <v>419</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>391</v>
+        <v>420</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>395</v>
+        <v>324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="43" t="s">
+        <v>595</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>396</v>
+        <v>610</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>437</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>390</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="D4" s="25"/>
       <c r="E4" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>421</v>
+    </row>
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="43" t="s">
+        <v>422</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>399</v>
@@ -9438,19 +9537,16 @@
       <c r="E5" s="25" t="s">
         <v>391</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>436</v>
+    </row>
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>596</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>400</v>
+        <v>408</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>390</v>
@@ -9459,178 +9555,174 @@
         <v>391</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>401</v>
+        <v>408</v>
+      </c>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="43" t="s">
+        <v>597</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>402</v>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>598</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>402</v>
+        <v>607</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>423</v>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
+        <v>392</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>437</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="E9" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>424</v>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>395</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>425</v>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>599</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>408</v>
+        <v>612</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>438</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>399</v>
+        <v>426</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>426</v>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>608</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>427</v>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="43" t="s">
+        <v>609</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>390</v>
+        <v>405</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>433</v>
+        <v>406</v>
+      </c>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>398</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>439</v>
+        <v>425</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>435</v>
+        <v>399</v>
       </c>
       <c r="E14" s="25" t="s">
         <v>391</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>430</v>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
+        <v>600</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>412</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D15" s="25" t="s">
         <v>413</v>
@@ -9642,15 +9734,15 @@
         <v>415</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>431</v>
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>601</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>416</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>390</v>
@@ -9661,28 +9753,143 @@
       <c r="F16" s="25" t="s">
         <v>416</v>
       </c>
+      <c r="G16" s="25"/>
     </row>
     <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>432</v>
+      <c r="A17" s="43" t="s">
+        <v>602</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>419</v>
+        <v>390</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>420</v>
+        <v>391</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>324</v>
-      </c>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
+        <v>401</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>424</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
+        <v>603</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>613</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
+        <v>604</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>616</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
+        <v>605</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>614</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="43" t="s">
+        <v>606</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>615</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>402</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B39" s="25"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
+    <sortCondition ref="A2:A23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9706,19 +9913,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -9726,16 +9933,16 @@
         <v>360</v>
       </c>
       <c r="B2" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="C2" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="D2" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="E2" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -9743,19 +9950,205 @@
         <v>361</v>
       </c>
       <c r="B3" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="C3" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="D3" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="E3" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874AFBB5-8FFB-B248-A4C3-9A81309B9614}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>595</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="45" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>395</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>608</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>609</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="44"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
+    <sortCondition ref="A2:A20"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed data error and regenerate the results table.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42B4C12-A117-6449-AE96-AD16BD61F039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F143C3EC-2C9E-154D-A5D0-3C78DBFC9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50440" yWindow="5140" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -2553,11 +2553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3947,10 +3947,10 @@
         <v>377</v>
       </c>
       <c r="H24" s="12">
-        <v>-81.1824412</v>
+        <v>-81.165005500000007</v>
       </c>
       <c r="I24" s="12">
-        <v>37.946477700000003</v>
+        <v>37.946770700000002</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>593</v>
@@ -7148,9 +7148,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8400,8 +8400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7DED6B-84CB-6D46-B3EB-C814548CEBA4}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Data update 2/16, and many changes to the dashboard.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F143C3EC-2C9E-154D-A5D0-3C78DBFC9460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D2F676-5D18-4E40-9C94-23AA03D22355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -2553,11 +2553,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2712,7 +2712,7 @@
         <v>360</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>68</v>
@@ -4031,7 +4031,7 @@
         <v>361</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>156</v>
@@ -4129,7 +4129,7 @@
         <v>361</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>68</v>
@@ -4183,7 +4183,7 @@
         <v>361</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>164</v>
@@ -4241,7 +4241,7 @@
         <v>361</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>160</v>
@@ -4299,7 +4299,7 @@
         <v>361</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>155</v>
@@ -4320,7 +4320,7 @@
         <v>362</v>
       </c>
       <c r="K31" s="29" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="L31" s="33">
         <v>56000</v>
@@ -4357,7 +4357,7 @@
         <v>361</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E32" s="29" t="s">
         <v>166</v>
@@ -4417,7 +4417,7 @@
         <v>361</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>170</v>
@@ -4477,7 +4477,7 @@
         <v>361</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>163</v>
@@ -4535,7 +4535,7 @@
         <v>361</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>179</v>
@@ -4595,7 +4595,7 @@
         <v>361</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>177</v>
@@ -7148,7 +7148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+    <sheetView zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>

</xml_diff>

<commit_message>
Major dashboard update and first prelim release
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D2F676-5D18-4E40-9C94-23AA03D22355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D6D88E-19CF-BE40-BA20-B470ADFD51B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
@@ -2557,7 +2557,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3760,8 +3760,8 @@
       <c r="C21" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>103</v>
+      <c r="D21" s="40" t="s">
+        <v>60</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
Minor data repair from MU.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F90087-76C2-F04B-9A5B-825240CD6600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B72292-9838-BA47-8870-E3972E546152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="647">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1874,112 +1874,112 @@
     <t>C3b</t>
   </si>
   <si>
-    <t>N1:SARS</t>
-  </si>
-  <si>
-    <t>N2:SARS</t>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>RNase P</t>
+  </si>
+  <si>
+    <t>S:E484K</t>
+  </si>
+  <si>
+    <t>S:E484K WT</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70</t>
+  </si>
+  <si>
+    <t>S:HVdel69-70 WT</t>
+  </si>
+  <si>
+    <t>S:N501Y</t>
+  </si>
+  <si>
+    <t>S:N501Y WT</t>
+  </si>
+  <si>
+    <t>TNFR</t>
+  </si>
+  <si>
+    <t>locus_id</t>
+  </si>
+  <si>
+    <t>SaltRock WWTP: Ona and SaltRock</t>
+  </si>
+  <si>
+    <t>SaltRock WWTP: Milton and Culloden</t>
+  </si>
+  <si>
+    <t>CharlestonWVU</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>Hometown-Putnam</t>
+  </si>
+  <si>
+    <t>PutnamPSD</t>
+  </si>
+  <si>
+    <t>3rdAndHalGreerMU</t>
+  </si>
+  <si>
+    <t>CommonsDormsMU</t>
+  </si>
+  <si>
+    <t>SRCM</t>
+  </si>
+  <si>
+    <t>TwinTowersEastDormMU</t>
+  </si>
+  <si>
+    <t>TwinTowersWestDormMU</t>
+  </si>
+  <si>
+    <t>MU HACH</t>
+  </si>
+  <si>
+    <t>Manhole collects from Willis, Gibson, and Wellman dormatories - Haymaker WW goes toward Harless Cafe</t>
+  </si>
+  <si>
+    <t>Manhole located on the corner of 3rd Avene and Hal Greer. Collects from parts or all of Smith Music Hall, Smith Hall, Communications Building, and Science Building, Morrow, and Old Main</t>
+  </si>
+  <si>
+    <t>Lagoon - plan to pump into PeaRidge some day when new pearidge plant comes to be</t>
+  </si>
+  <si>
+    <t>Upstream from Huntington Sanitary board</t>
+  </si>
+  <si>
+    <t>Small independent plant under PeaRidge management</t>
+  </si>
+  <si>
+    <t>HometownWWTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54079-002-01-00-00</t>
+  </si>
+  <si>
+    <t>Putnam PSD</t>
+  </si>
+  <si>
+    <t>WV0028045</t>
+  </si>
+  <si>
+    <t>Human</t>
   </si>
   <si>
     <t>NEP/NS1</t>
   </si>
   <si>
-    <t>POL</t>
-  </si>
-  <si>
-    <t>RNase P</t>
-  </si>
-  <si>
-    <t>S:E484K</t>
-  </si>
-  <si>
-    <t>S:E484K WT</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70</t>
-  </si>
-  <si>
-    <t>S:HVdel69-70 WT</t>
-  </si>
-  <si>
-    <t>S:N501Y</t>
-  </si>
-  <si>
-    <t>S:N501Y WT</t>
-  </si>
-  <si>
-    <t>TNFR</t>
-  </si>
-  <si>
-    <t>locus_id</t>
-  </si>
-  <si>
-    <t>SaltRock WWTP: Ona and SaltRock</t>
-  </si>
-  <si>
-    <t>SaltRock WWTP: Milton and Culloden</t>
-  </si>
-  <si>
-    <t>CharlestonWVU</t>
-  </si>
-  <si>
-    <t>PUT</t>
-  </si>
-  <si>
-    <t>Hometown-Putnam</t>
-  </si>
-  <si>
-    <t>PutnamPSD</t>
-  </si>
-  <si>
-    <t>3rdAndHalGreerMU</t>
-  </si>
-  <si>
-    <t>CommonsDormsMU</t>
-  </si>
-  <si>
-    <t>SRCM</t>
-  </si>
-  <si>
-    <t>TwinTowersEastDormMU</t>
-  </si>
-  <si>
-    <t>TwinTowersWestDormMU</t>
-  </si>
-  <si>
-    <t>MU HACH</t>
-  </si>
-  <si>
-    <t>Manhole collects from Willis, Gibson, and Wellman dormatories - Haymaker WW goes toward Harless Cafe</t>
-  </si>
-  <si>
-    <t>Manhole located on the corner of 3rd Avene and Hal Greer. Collects from parts or all of Smith Music Hall, Smith Hall, Communications Building, and Science Building, Morrow, and Old Main</t>
-  </si>
-  <si>
-    <t>Lagoon - plan to pump into PeaRidge some day when new pearidge plant comes to be</t>
-  </si>
-  <si>
-    <t>Upstream from Huntington Sanitary board</t>
-  </si>
-  <si>
-    <t>Small independent plant under PeaRidge management</t>
-  </si>
-  <si>
-    <t>HometownWWTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 54079-002-01-00-00</t>
-  </si>
-  <si>
-    <t>Putnam PSD</t>
-  </si>
-  <si>
-    <t>WV0028045</t>
-  </si>
-  <si>
-    <t>M:FLUA</t>
-  </si>
-  <si>
-    <t>Human</t>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>SC2</t>
   </si>
 </sst>
 </file>
@@ -2784,7 +2784,7 @@
         <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>340</v>
@@ -4080,14 +4080,14 @@
         <v>38.424089000000002</v>
       </c>
       <c r="J25" s="46" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L25" s="33"/>
       <c r="M25" s="33" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N25" s="33">
         <v>5</v>
@@ -4108,7 +4108,7 @@
         <v>25703</v>
       </c>
       <c r="T25" s="46" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4147,7 +4147,7 @@
         <v>4000</v>
       </c>
       <c r="M26" s="33" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N26" s="33">
         <v>24</v>
@@ -4168,7 +4168,7 @@
         <v>25504</v>
       </c>
       <c r="T26" s="47" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="27" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4198,14 +4198,14 @@
         <v>38.421745999999999</v>
       </c>
       <c r="J27" s="46" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="K27" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L27" s="33"/>
       <c r="M27" s="33" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N27" s="33">
         <v>5</v>
@@ -4226,7 +4226,7 @@
         <v>25703</v>
       </c>
       <c r="T27" s="46" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="28" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -4514,7 +4514,7 @@
         <v>25701</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4574,7 +4574,7 @@
         <v>25537</v>
       </c>
       <c r="T33" s="29" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="34" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4613,7 +4613,7 @@
         <v>7000</v>
       </c>
       <c r="M34" s="34" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N34" s="34">
         <v>24</v>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="29" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B35" s="29"/>
       <c r="C35" s="29" t="s">
@@ -4647,7 +4647,7 @@
         <v>103</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="F35" s="29" t="s">
         <v>340</v>
@@ -4707,7 +4707,7 @@
         <v>103</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="F36" s="29" t="s">
         <v>340</v>
@@ -4782,14 +4782,14 @@
         <v>38.422913110104098</v>
       </c>
       <c r="J37" s="46" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="K37" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="34" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N37" s="33">
         <v>5</v>
@@ -4838,14 +4838,14 @@
         <v>38.423076174075902</v>
       </c>
       <c r="J38" s="46" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="K38" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L38" s="33"/>
       <c r="M38" s="34" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="N38" s="33">
         <v>24</v>
@@ -4869,7 +4869,7 @@
     </row>
     <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="46" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="B39" s="46"/>
       <c r="C39" s="46" t="s">
@@ -4879,7 +4879,7 @@
         <v>103</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="F39" s="46" t="s">
         <v>340</v>
@@ -4894,7 +4894,7 @@
         <v>38.537901317549398</v>
       </c>
       <c r="J39" s="46" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="K39" s="46" t="s">
         <v>159</v>
@@ -8594,22 +8594,22 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B47" s="52" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C47" s="51" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D47" s="51" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E47" s="51" t="s">
         <v>159</v>
       </c>
       <c r="F47" s="51" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="G47" s="51"/>
       <c r="H47" s="51">
@@ -9679,7 +9679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
@@ -10219,8 +10219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874AFBB5-8FFB-B248-A4C3-9A81309B9614}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -10235,7 +10235,7 @@
         <v>374</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -10248,10 +10248,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -10259,7 +10259,7 @@
         <v>383</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>645</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -10267,7 +10267,7 @@
         <v>386</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>613</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -10291,7 +10291,7 @@
         <v>600</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -10299,7 +10299,7 @@
         <v>389</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -10323,7 +10323,7 @@
         <v>393</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>611</v>
+        <v>644</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -10331,7 +10331,7 @@
         <v>393</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>612</v>
+        <v>645</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10339,7 +10339,7 @@
         <v>393</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>335</v>
+        <v>646</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10347,7 +10347,7 @@
         <v>393</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>616</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10355,7 +10355,7 @@
         <v>393</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -10363,7 +10363,7 @@
         <v>393</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10371,7 +10371,7 @@
         <v>393</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10379,7 +10379,7 @@
         <v>393</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10387,11 +10387,16 @@
         <v>393</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
+      <c r="A21" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>618</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">

</xml_diff>

<commit_message>
Added Norovirus tab. Still need to add warning block about no data, via hidden panel method. But it works for now.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1B925E-7564-E844-BB72-3B253306D3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA468563-08FF-834B-9CC4-BAF89E358689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19780" yWindow="500" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="652">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1993,6 +1993,9 @@
   </si>
   <si>
     <t>Nanotrap concentration of raw influent and quantification by ddPCR; the only modification from major_lab_method 1 is that post-RNA extraction, three equal volumes of RNA extract are combined for ddPCR analysis, rather than being combined pre-concentration.</t>
+  </si>
+  <si>
+    <t>huNovGI</t>
   </si>
 </sst>
 </file>
@@ -2649,7 +2652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9704,11 +9707,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9971,10 +9974,10 @@
     </row>
     <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>389</v>
+        <v>644</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>412</v>
+        <v>651</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>416</v>
@@ -9991,51 +9994,50 @@
     </row>
     <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
-        <v>591</v>
+        <v>641</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>416</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>416</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>381</v>
+        <v>404</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F16" s="25" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
+        <v>592</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>407</v>
-      </c>
-      <c r="G16" s="25"/>
-    </row>
-    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>593</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>391</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>416</v>
@@ -10044,18 +10046,19 @@
         <v>381</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>382</v>
+        <v>408</v>
       </c>
       <c r="F17" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="43" t="s">
+        <v>593</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
-        <v>392</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>415</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>416</v>
@@ -10067,32 +10070,35 @@
         <v>382</v>
       </c>
       <c r="F18" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="43" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
-        <v>594</v>
-      </c>
       <c r="B19" s="25" t="s">
-        <v>603</v>
+        <v>415</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="E19" s="25" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="F19" s="25" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>417</v>
@@ -10104,12 +10110,12 @@
         <v>382</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>417</v>
@@ -10121,12 +10127,12 @@
         <v>382</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>417</v>
@@ -10138,32 +10144,49 @@
         <v>382</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>393</v>
+        <v>597</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>393</v>
+        <v>605</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="E23" s="25" t="s">
         <v>382</v>
       </c>
-      <c r="F23" s="25" t="s">
+    </row>
+    <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>393</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>416</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="F24" s="25" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="B39" s="25"/>
+    <row r="40" spans="2:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B40" s="25"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
-    <sortCondition ref="A2:A23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F24">
+    <sortCondition ref="A2:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new site Moorefield to the watch tables.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA468563-08FF-834B-9CC4-BAF89E358689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93A5CFF-A093-CD45-BF2F-CFF979B15785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="51960" yWindow="4820" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="625">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1344,105 +1344,6 @@
     <t>V</t>
   </si>
   <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>EE</t>
-  </si>
-  <si>
-    <t>FF</t>
-  </si>
-  <si>
-    <t>GG</t>
-  </si>
-  <si>
-    <t>HH</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>JJ</t>
-  </si>
-  <si>
-    <t>KK</t>
-  </si>
-  <si>
-    <t>LL</t>
-  </si>
-  <si>
-    <t>MM</t>
-  </si>
-  <si>
-    <t>NN</t>
-  </si>
-  <si>
-    <t>OO</t>
-  </si>
-  <si>
-    <t>PP</t>
-  </si>
-  <si>
-    <t>QQ</t>
-  </si>
-  <si>
-    <t>RR</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>TT</t>
-  </si>
-  <si>
-    <t>UU</t>
-  </si>
-  <si>
-    <t>VV</t>
-  </si>
-  <si>
-    <t>WW</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>YY</t>
-  </si>
-  <si>
-    <t>ZZ</t>
-  </si>
-  <si>
-    <t>AAA</t>
-  </si>
-  <si>
-    <t>BBB</t>
-  </si>
-  <si>
-    <t>CCC</t>
-  </si>
-  <si>
     <t>StadiumSW-01</t>
   </si>
   <si>
@@ -1996,6 +1897,24 @@
   </si>
   <si>
     <t>huNovGI</t>
+  </si>
+  <si>
+    <t>MoorefieldWWTP-01</t>
+  </si>
+  <si>
+    <t>Moorefield</t>
+  </si>
+  <si>
+    <t>MoorefieldWWTP</t>
+  </si>
+  <si>
+    <t>Moorefield WWTP</t>
+  </si>
+  <si>
+    <t>V01</t>
+  </si>
+  <si>
+    <t>54029-001-01-00-00</t>
   </si>
 </sst>
 </file>
@@ -2005,7 +1924,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2158,6 +2077,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2204,7 +2128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2329,6 +2253,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2650,13 +2586,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:T81"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D64" sqref="D61:D64"/>
+      <selection pane="bottomRight" activeCell="Q82" sqref="Q82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2683,7 +2619,7 @@
         <v>191</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>541</v>
+        <v>508</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>349</v>
@@ -2946,7 +2882,7 @@
         <v>7000</v>
       </c>
       <c r="M5" s="34" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N5" s="34">
         <v>24</v>
@@ -2970,7 +2906,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
-        <v>618</v>
+        <v>585</v>
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="45" t="s">
@@ -2980,7 +2916,7 @@
         <v>103</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>619</v>
+        <v>586</v>
       </c>
       <c r="F6" s="45" t="s">
         <v>340</v>
@@ -2995,7 +2931,7 @@
         <v>38.537901317549398</v>
       </c>
       <c r="J6" s="45" t="s">
-        <v>620</v>
+        <v>587</v>
       </c>
       <c r="K6" s="45" t="s">
         <v>159</v>
@@ -3028,7 +2964,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
-        <v>623</v>
+        <v>590</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="29" t="s">
@@ -3038,7 +2974,7 @@
         <v>103</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>616</v>
+        <v>583</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>340</v>
@@ -3098,7 +3034,7 @@
         <v>103</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>615</v>
+        <v>582</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>340</v>
@@ -3151,7 +3087,7 @@
         <v>62</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>542</v>
+        <v>509</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>351</v>
@@ -3212,7 +3148,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>567</v>
+        <v>534</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>351</v>
@@ -3268,7 +3204,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>568</v>
+        <v>535</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>351</v>
@@ -3328,7 +3264,7 @@
         <v>93</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>549</v>
+        <v>516</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>351</v>
@@ -3381,10 +3317,10 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>351</v>
@@ -3393,7 +3329,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>476</v>
+        <v>443</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>341</v>
@@ -3442,7 +3378,7 @@
         <v>113</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>550</v>
+        <v>517</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>351</v>
@@ -3502,7 +3438,7 @@
         <v>109</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>583</v>
+        <v>550</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>351</v>
@@ -3562,7 +3498,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>553</v>
+        <v>520</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>351</v>
@@ -3618,7 +3554,7 @@
         <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>554</v>
+        <v>521</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>351</v>
@@ -3678,7 +3614,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>555</v>
+        <v>522</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>351</v>
@@ -3738,7 +3674,7 @@
         <v>152</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>556</v>
+        <v>523</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>351</v>
@@ -3798,7 +3734,7 @@
         <v>104</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>551</v>
+        <v>518</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>351</v>
@@ -3858,7 +3794,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>557</v>
+        <v>524</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>351</v>
@@ -3913,7 +3849,7 @@
         <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>558</v>
+        <v>525</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>351</v>
@@ -3969,7 +3905,7 @@
         <v>188</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>559</v>
+        <v>526</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>351</v>
@@ -4028,7 +3964,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>561</v>
+        <v>528</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>351</v>
@@ -4088,7 +4024,7 @@
         <v>106</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>562</v>
+        <v>529</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>351</v>
@@ -4147,7 +4083,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>544</v>
+        <v>511</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>351</v>
@@ -4203,7 +4139,7 @@
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>558</v>
+        <v>525</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>351</v>
@@ -4263,7 +4199,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>566</v>
+        <v>533</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>351</v>
@@ -4316,10 +4252,10 @@
     </row>
     <row r="29" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>477</v>
+        <v>444</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>543</v>
+        <v>510</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>351</v>
@@ -4328,7 +4264,7 @@
         <v>103</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>478</v>
+        <v>445</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>340</v>
@@ -4343,7 +4279,7 @@
         <v>37.946770700000002</v>
       </c>
       <c r="J29" s="12" t="s">
-        <v>584</v>
+        <v>551</v>
       </c>
       <c r="K29" s="12" t="s">
         <v>197</v>
@@ -4401,14 +4337,14 @@
         <v>38.424089000000002</v>
       </c>
       <c r="J30" s="45" t="s">
-        <v>621</v>
+        <v>588</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L30" s="33"/>
       <c r="M30" s="33" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N30" s="33">
         <v>5</v>
@@ -4429,7 +4365,7 @@
         <v>25703</v>
       </c>
       <c r="T30" s="45" t="s">
-        <v>628</v>
+        <v>595</v>
       </c>
     </row>
     <row r="31" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4468,7 +4404,7 @@
         <v>4000</v>
       </c>
       <c r="M31" s="33" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N31" s="33">
         <v>24</v>
@@ -4489,7 +4425,7 @@
         <v>25504</v>
       </c>
       <c r="T31" s="46" t="s">
-        <v>629</v>
+        <v>596</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
@@ -4519,14 +4455,14 @@
         <v>38.421745999999999</v>
       </c>
       <c r="J32" s="45" t="s">
-        <v>622</v>
+        <v>589</v>
       </c>
       <c r="K32" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L32" s="33"/>
       <c r="M32" s="33" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N32" s="33">
         <v>5</v>
@@ -4547,7 +4483,7 @@
         <v>25703</v>
       </c>
       <c r="T32" s="45" t="s">
-        <v>627</v>
+        <v>594</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -4665,7 +4601,7 @@
         <v>25701</v>
       </c>
       <c r="T34" s="29" t="s">
-        <v>630</v>
+        <v>597</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -4725,7 +4661,7 @@
         <v>25537</v>
       </c>
       <c r="T35" s="29" t="s">
-        <v>631</v>
+        <v>598</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
@@ -4755,14 +4691,14 @@
         <v>38.422913110104098</v>
       </c>
       <c r="J36" s="45" t="s">
-        <v>624</v>
+        <v>591</v>
       </c>
       <c r="K36" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L36" s="33"/>
       <c r="M36" s="34" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N36" s="33">
         <v>5</v>
@@ -4811,14 +4747,14 @@
         <v>38.423076174075902</v>
       </c>
       <c r="J37" s="45" t="s">
-        <v>625</v>
+        <v>592</v>
       </c>
       <c r="K37" s="29" t="s">
         <v>157</v>
       </c>
       <c r="L37" s="33"/>
       <c r="M37" s="34" t="s">
-        <v>626</v>
+        <v>593</v>
       </c>
       <c r="N37" s="33">
         <v>24</v>
@@ -4845,7 +4781,7 @@
         <v>18</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>547</v>
+        <v>514</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>351</v>
@@ -4905,7 +4841,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>351</v>
@@ -4961,7 +4897,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>548</v>
+        <v>515</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>351</v>
@@ -4970,7 +4906,7 @@
         <v>60</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>617</v>
+        <v>584</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>340</v>
@@ -5017,7 +4953,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>351</v>
@@ -5073,7 +5009,7 @@
         <v>21</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>351</v>
@@ -5135,7 +5071,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>351</v>
@@ -5197,7 +5133,7 @@
         <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>351</v>
@@ -5259,7 +5195,7 @@
         <v>22</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>351</v>
@@ -5319,7 +5255,7 @@
         <v>27</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>351</v>
@@ -5379,7 +5315,7 @@
         <v>28</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>351</v>
@@ -5439,7 +5375,7 @@
         <v>111</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>552</v>
+        <v>519</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>351</v>
@@ -5550,7 +5486,7 @@
         <v>192</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>351</v>
@@ -5612,7 +5548,7 @@
         <v>29</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>351</v>
@@ -5672,7 +5608,7 @@
         <v>30</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>351</v>
@@ -5732,7 +5668,7 @@
         <v>38</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>351</v>
@@ -5787,7 +5723,7 @@
         <v>39</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>351</v>
@@ -5842,7 +5778,7 @@
         <v>31</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>351</v>
@@ -5902,7 +5838,7 @@
         <v>36</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>351</v>
@@ -5957,7 +5893,7 @@
         <v>339</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>351</v>
@@ -6017,7 +5953,7 @@
         <v>23</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>351</v>
@@ -6133,7 +6069,7 @@
         <v>184</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>351</v>
@@ -6192,10 +6128,10 @@
     </row>
     <row r="61" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>471</v>
+        <v>438</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>351</v>
@@ -6204,7 +6140,7 @@
         <v>103</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>472</v>
+        <v>439</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>341</v>
@@ -6246,10 +6182,10 @@
     </row>
     <row r="62" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>351</v>
@@ -6258,7 +6194,7 @@
         <v>103</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>470</v>
+        <v>437</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>341</v>
@@ -6300,10 +6236,10 @@
     </row>
     <row r="63" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>473</v>
+        <v>440</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>351</v>
@@ -6312,7 +6248,7 @@
         <v>103</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>474</v>
+        <v>441</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>341</v>
@@ -6354,10 +6290,10 @@
     </row>
     <row r="64" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>467</v>
+        <v>434</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>351</v>
@@ -6366,7 +6302,7 @@
         <v>103</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>468</v>
+        <v>435</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>341</v>
@@ -6411,7 +6347,7 @@
         <v>51</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>563</v>
+        <v>530</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>351</v>
@@ -6471,7 +6407,7 @@
         <v>58</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>351</v>
@@ -6527,7 +6463,7 @@
         <v>24</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>351</v>
@@ -6589,7 +6525,7 @@
         <v>37</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>546</v>
+        <v>513</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>351</v>
@@ -6645,7 +6581,7 @@
         <v>32</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>351</v>
@@ -6705,7 +6641,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>565</v>
+        <v>532</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>351</v>
@@ -6765,7 +6701,7 @@
         <v>33</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>545</v>
+        <v>512</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>351</v>
@@ -7103,7 +7039,7 @@
         <v>59</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>560</v>
+        <v>527</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>351</v>
@@ -7211,7 +7147,7 @@
         <v>14</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>564</v>
+        <v>531</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>351</v>
@@ -7366,6 +7302,50 @@
         <v>26591</v>
       </c>
       <c r="T81" s="2"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="B82" t="s">
+        <v>623</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="H82" s="2">
+        <v>-78.955160000000006</v>
+      </c>
+      <c r="I82" s="2">
+        <v>39.115929999999999</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L82" s="38">
+        <v>3510</v>
+      </c>
+      <c r="R82" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S82" s="1">
+        <v>26836</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T81">
@@ -7379,16 +7359,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" customWidth="1"/>
     <col min="4" max="5" width="23.83203125" customWidth="1"/>
@@ -7403,7 +7383,7 @@
         <v>230</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>504</v>
+        <v>471</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>229</v>
@@ -7415,7 +7395,7 @@
         <v>238</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>480</v>
+        <v>447</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>240</v>
@@ -7432,7 +7412,7 @@
         <v>275</v>
       </c>
       <c r="B2" t="s">
-        <v>505</v>
+        <v>472</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>64</v>
@@ -7444,7 +7424,7 @@
         <v>63</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>481</v>
+        <v>448</v>
       </c>
       <c r="G2" s="31">
         <v>54003906001</v>
@@ -7462,7 +7442,7 @@
         <v>244</v>
       </c>
       <c r="B3" t="s">
-        <v>506</v>
+        <v>473</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>277</v>
@@ -7474,7 +7454,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>482</v>
+        <v>449</v>
       </c>
       <c r="G3" s="17">
         <v>54002701001</v>
@@ -7499,7 +7479,7 @@
         <v>157</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>573</v>
+        <v>540</v>
       </c>
       <c r="G4" s="31">
         <v>54000601001</v>
@@ -7526,7 +7506,7 @@
         <v>123</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>574</v>
+        <v>541</v>
       </c>
       <c r="G5" s="31">
         <v>54000101001</v>
@@ -7553,7 +7533,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>575</v>
+        <v>542</v>
       </c>
       <c r="G6" s="31">
         <v>54003031001</v>
@@ -7580,7 +7560,7 @@
         <v>88</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>576</v>
+        <v>543</v>
       </c>
       <c r="G7" s="31">
         <v>54001702001</v>
@@ -7605,7 +7585,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>577</v>
+        <v>544</v>
       </c>
       <c r="G8" s="31">
         <v>54002510001</v>
@@ -7622,7 +7602,7 @@
         <v>357</v>
       </c>
       <c r="B9" t="s">
-        <v>508</v>
+        <v>475</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>362</v>
@@ -7632,7 +7612,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>536</v>
+        <v>503</v>
       </c>
       <c r="G9" s="31">
         <v>54002003001</v>
@@ -7649,7 +7629,7 @@
         <v>249</v>
       </c>
       <c r="B10" t="s">
-        <v>507</v>
+        <v>474</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>282</v>
@@ -7659,7 +7639,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>483</v>
+        <v>450</v>
       </c>
       <c r="G10" s="31">
         <v>54002003001</v>
@@ -7676,7 +7656,7 @@
         <v>250</v>
       </c>
       <c r="B11" t="s">
-        <v>509</v>
+        <v>476</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>283</v>
@@ -7686,7 +7666,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>484</v>
+        <v>451</v>
       </c>
       <c r="G11" s="31">
         <v>54001901001</v>
@@ -7703,7 +7683,7 @@
         <v>251</v>
       </c>
       <c r="B12" t="s">
-        <v>510</v>
+        <v>477</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>306</v>
@@ -7715,7 +7695,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>485</v>
+        <v>452</v>
       </c>
       <c r="G12" s="31">
         <v>54003045001</v>
@@ -7732,7 +7712,7 @@
         <v>252</v>
       </c>
       <c r="B13" t="s">
-        <v>511</v>
+        <v>478</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>284</v>
@@ -7742,7 +7722,7 @@
         <v>88</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>486</v>
+        <v>453</v>
       </c>
       <c r="G13" s="31">
         <v>54001703001</v>
@@ -7759,7 +7739,7 @@
         <v>358</v>
       </c>
       <c r="B14" t="s">
-        <v>512</v>
+        <v>479</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>363</v>
@@ -7769,7 +7749,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>537</v>
+        <v>504</v>
       </c>
       <c r="G14" s="31">
         <v>54002007001</v>
@@ -7786,7 +7766,7 @@
         <v>253</v>
       </c>
       <c r="B15" t="s">
-        <v>513</v>
+        <v>480</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>285</v>
@@ -7796,7 +7776,7 @@
         <v>121</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>487</v>
+        <v>454</v>
       </c>
       <c r="G15" s="31">
         <v>54004202001</v>
@@ -7821,7 +7801,7 @@
         <v>89</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>578</v>
+        <v>545</v>
       </c>
       <c r="G16" s="31">
         <v>54002405001</v>
@@ -7838,7 +7818,7 @@
         <v>255</v>
       </c>
       <c r="B17" t="s">
-        <v>514</v>
+        <v>481</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>287</v>
@@ -7848,7 +7828,7 @@
         <v>89</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>579</v>
+        <v>546</v>
       </c>
       <c r="G17" s="31">
         <v>54002408001</v>
@@ -7865,7 +7845,7 @@
         <v>256</v>
       </c>
       <c r="B18" t="s">
-        <v>515</v>
+        <v>482</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>288</v>
@@ -7875,7 +7855,7 @@
         <v>122</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>488</v>
+        <v>455</v>
       </c>
       <c r="G18" s="17">
         <v>54000504001</v>
@@ -7892,7 +7872,7 @@
         <v>257</v>
       </c>
       <c r="B19" t="s">
-        <v>516</v>
+        <v>483</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>289</v>
@@ -7902,7 +7882,7 @@
         <v>100</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>489</v>
+        <v>456</v>
       </c>
       <c r="G19" s="31">
         <v>54004602001</v>
@@ -7938,240 +7918,246 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="B21" t="s">
-        <v>517</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="F21" t="s">
-        <v>538</v>
-      </c>
-      <c r="G21" s="31">
-        <v>54000603001</v>
-      </c>
-      <c r="H21" s="17">
-        <v>17</v>
-      </c>
-      <c r="I21" s="17">
-        <v>56000</v>
+      <c r="A21" s="50" t="s">
+        <v>599</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>600</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>586</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>601</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="50" t="s">
+        <v>602</v>
+      </c>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50">
+        <v>0.3</v>
+      </c>
+      <c r="I21" s="52">
+        <v>3500</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>258</v>
+        <v>353</v>
       </c>
       <c r="B22" t="s">
-        <v>518</v>
+        <v>484</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="D22" s="17"/>
+        <v>360</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>361</v>
+      </c>
       <c r="E22" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>490</v>
+        <v>182</v>
+      </c>
+      <c r="F22" t="s">
+        <v>505</v>
       </c>
       <c r="G22" s="31">
-        <v>54004215001</v>
+        <v>54000603001</v>
       </c>
       <c r="H22" s="17">
-        <v>0.41</v>
-      </c>
-      <c r="I22" s="30">
-        <v>2101</v>
+        <v>17</v>
+      </c>
+      <c r="I22" s="17">
+        <v>56000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="B23" t="s">
-        <v>519</v>
+        <v>485</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>580</v>
+        <v>457</v>
       </c>
       <c r="G23" s="31">
-        <v>54002803001</v>
+        <v>54004215001</v>
       </c>
       <c r="H23" s="17">
-        <v>2.4</v>
+        <v>0.41</v>
       </c>
       <c r="I23" s="30">
-        <v>8168</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="B24" t="s">
-        <v>520</v>
+        <v>486</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>491</v>
+        <v>547</v>
       </c>
       <c r="G24" s="31">
-        <v>54000316001</v>
+        <v>54002803001</v>
       </c>
       <c r="H24" s="17">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
       <c r="I24" s="30">
-        <v>4555</v>
+        <v>8168</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B25" t="s">
-        <v>521</v>
+        <v>487</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>492</v>
+        <v>458</v>
       </c>
       <c r="G25" s="31">
-        <v>54002415001</v>
+        <v>54000316001</v>
       </c>
       <c r="H25" s="17">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I25" s="30">
-        <v>1091</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B26" t="s">
-        <v>522</v>
+        <v>488</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="17" t="s">
-        <v>5</v>
+        <v>89</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>493</v>
+        <v>459</v>
       </c>
       <c r="G26" s="31">
-        <v>54002509001</v>
+        <v>54002415001</v>
       </c>
       <c r="H26" s="17">
-        <v>2.34</v>
+        <v>0.25</v>
       </c>
       <c r="I26" s="30">
-        <v>12000</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B27" t="s">
-        <v>523</v>
+        <v>489</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>494</v>
+        <v>460</v>
       </c>
       <c r="G27" s="31">
-        <v>54005405001</v>
+        <v>54002509001</v>
       </c>
       <c r="H27" s="17">
-        <v>15.5</v>
+        <v>2.34</v>
       </c>
       <c r="I27" s="30">
-        <v>48050</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>355</v>
+        <v>262</v>
       </c>
       <c r="B28" t="s">
-        <v>524</v>
+        <v>490</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>365</v>
+        <v>296</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" t="s">
-        <v>539</v>
-      </c>
-      <c r="G28" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="G28" s="31">
+        <v>54005405001</v>
+      </c>
       <c r="H28" s="17">
-        <v>2.16</v>
-      </c>
-      <c r="I28" s="17">
-        <v>7000</v>
+        <v>15.5</v>
+      </c>
+      <c r="I28" s="30">
+        <v>48050</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="B29" s="17"/>
+        <v>355</v>
+      </c>
+      <c r="B29" t="s">
+        <v>491</v>
+      </c>
       <c r="C29" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
+      <c r="F29" t="s">
+        <v>506</v>
+      </c>
+      <c r="G29" s="4"/>
       <c r="H29" s="17">
-        <v>0.125</v>
+        <v>2.16</v>
       </c>
       <c r="I29" s="17">
-        <v>1000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -8182,437 +8168,435 @@
       <c r="C30" s="17" t="s">
         <v>366</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="17" t="s">
         <v>157</v>
       </c>
       <c r="F30" s="17"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4">
+      <c r="G30" s="17"/>
+      <c r="H30" s="17">
         <v>0.125</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="17">
         <v>1000</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>263</v>
+        <v>354</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="D31" s="17"/>
+        <v>366</v>
+      </c>
+      <c r="D31" s="4"/>
       <c r="E31" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="17" t="s">
-        <v>572</v>
-      </c>
-      <c r="G31" s="17">
-        <v>54001205001</v>
-      </c>
-      <c r="H31" s="17">
-        <v>1.35</v>
-      </c>
-      <c r="I31" s="30">
-        <v>2700</v>
+        <v>157</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="B32" t="s">
-        <v>525</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B32" s="17"/>
       <c r="C32" s="17" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>495</v>
+        <v>55</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>539</v>
       </c>
       <c r="G32" s="17">
-        <v>54002606001</v>
+        <v>54001205001</v>
       </c>
       <c r="H32" s="17">
-        <v>0.7</v>
+        <v>1.35</v>
       </c>
       <c r="I32" s="30">
-        <v>5515</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s">
-        <v>526</v>
+        <v>492</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>496</v>
+        <v>462</v>
       </c>
       <c r="G33" s="17">
-        <v>54002716001</v>
+        <v>54002606001</v>
       </c>
       <c r="H33" s="17">
-        <v>4.9000000000000004</v>
+        <v>0.7</v>
       </c>
       <c r="I33" s="30">
-        <v>36000</v>
+        <v>5515</v>
       </c>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B34" t="s">
-        <v>527</v>
+        <v>493</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17" t="s">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>497</v>
-      </c>
-      <c r="G34" s="31">
-        <v>54001710001</v>
+        <v>463</v>
+      </c>
+      <c r="G34" s="17">
+        <v>54002716001</v>
       </c>
       <c r="H34" s="17">
-        <v>0.4</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I34" s="30">
-        <v>1853</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>370</v>
+        <v>266</v>
       </c>
       <c r="B35" t="s">
-        <v>528</v>
+        <v>494</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>372</v>
+        <v>299</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F35" t="s">
-        <v>540</v>
-      </c>
-      <c r="G35" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G35" s="31">
+        <v>54001710001</v>
+      </c>
       <c r="H35" s="17">
-        <v>1.8</v>
-      </c>
-      <c r="I35" s="17">
-        <v>7200</v>
+        <v>0.4</v>
+      </c>
+      <c r="I35" s="30">
+        <v>1853</v>
       </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B36" t="s">
-        <v>529</v>
+        <v>495</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17" t="s">
         <v>157</v>
       </c>
       <c r="F36" t="s">
-        <v>540</v>
-      </c>
-      <c r="G36" s="17"/>
+        <v>507</v>
+      </c>
+      <c r="G36" s="4"/>
       <c r="H36" s="17">
-        <v>0.7</v>
+        <v>1.8</v>
       </c>
       <c r="I36" s="17">
-        <v>4050</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="B37" s="17"/>
+        <v>371</v>
+      </c>
+      <c r="B37" t="s">
+        <v>496</v>
+      </c>
       <c r="C37" s="17" t="s">
-        <v>300</v>
+        <v>373</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>581</v>
-      </c>
-      <c r="G37" s="31">
-        <v>54004804001</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F37" t="s">
+        <v>507</v>
+      </c>
+      <c r="G37" s="17"/>
       <c r="H37" s="17">
-        <v>0.3</v>
-      </c>
-      <c r="I37" s="30">
-        <v>1800</v>
+        <v>0.7</v>
+      </c>
+      <c r="I37" s="17">
+        <v>4050</v>
       </c>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="B38" t="s">
-        <v>530</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="B38" s="17"/>
       <c r="C38" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>311</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="D38" s="17"/>
       <c r="E38" s="17" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>498</v>
+        <v>548</v>
       </c>
       <c r="G38" s="31">
-        <v>54003011001</v>
+        <v>54004804001</v>
       </c>
       <c r="H38" s="17">
-        <v>20.8</v>
+        <v>0.3</v>
       </c>
       <c r="I38" s="30">
-        <v>48328</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
       <c r="B39" t="s">
-        <v>531</v>
+        <v>497</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="D39" s="17"/>
+        <v>276</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>311</v>
+      </c>
       <c r="E39" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="17" t="s">
-        <v>582</v>
-      </c>
-      <c r="G39" s="17">
-        <v>54003703001</v>
+        <v>11</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="G39" s="31">
+        <v>54003011001</v>
       </c>
       <c r="H39" s="17">
-        <v>0.52500000000000002</v>
+        <v>20.8</v>
       </c>
       <c r="I39" s="30">
-        <v>2892</v>
+        <v>48328</v>
       </c>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B40" t="s">
-        <v>532</v>
+        <v>498</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>570</v>
-      </c>
-      <c r="G40" s="31">
-        <v>54003203001</v>
+        <v>549</v>
+      </c>
+      <c r="G40" s="17">
+        <v>54003703001</v>
       </c>
       <c r="H40" s="17">
-        <v>1.8</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="I40" s="30">
-        <v>3255</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="B41" s="17"/>
+        <v>269</v>
+      </c>
+      <c r="B41" t="s">
+        <v>499</v>
+      </c>
       <c r="C41" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="17" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>571</v>
+        <v>537</v>
       </c>
       <c r="G41" s="31">
-        <v>54000509001</v>
+        <v>54003203001</v>
       </c>
       <c r="H41" s="17">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="I41" s="30">
-        <v>20411</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="B42" t="s">
-        <v>533</v>
-      </c>
+        <v>270</v>
+      </c>
+      <c r="B42" s="17"/>
       <c r="C42" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17" t="s">
-        <v>9</v>
+        <v>122</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>499</v>
-      </c>
-      <c r="G42" s="17">
-        <v>54002102001</v>
+        <v>538</v>
+      </c>
+      <c r="G42" s="31">
+        <v>54000509001</v>
       </c>
       <c r="H42" s="17">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I42" s="30">
-        <v>10364</v>
+        <v>20411</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B43" t="s">
-        <v>534</v>
+        <v>500</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>500</v>
-      </c>
-      <c r="G43" s="31">
-        <v>54000901001</v>
+        <v>9</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="G43" s="17">
+        <v>54002102001</v>
       </c>
       <c r="H43" s="17">
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="I43" s="30">
-        <v>564</v>
+        <v>10364</v>
       </c>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B44" t="s">
-        <v>535</v>
+        <v>501</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="G44" s="31">
+        <v>54000901001</v>
+      </c>
+      <c r="H44" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="I44" s="30">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B45" t="s">
+        <v>502</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>501</v>
-      </c>
-      <c r="G44" s="31">
+      <c r="F45" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="G45" s="31">
         <v>54003508001</v>
       </c>
-      <c r="H44" s="17">
+      <c r="H45" s="17">
         <v>10</v>
       </c>
-      <c r="I44" s="30">
+      <c r="I45" s="30">
         <v>33782</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>569</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>479</v>
-      </c>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4" t="s">
+    <row r="46" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F45" s="31" t="s">
-        <v>502</v>
-      </c>
-      <c r="G45" s="31">
+      <c r="F46" s="31" t="s">
+        <v>469</v>
+      </c>
+      <c r="G46" s="31">
         <v>54001022001</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H46" s="4">
         <v>0.75</v>
       </c>
-      <c r="I45" s="19">
+      <c r="I46" s="19">
         <v>2626</v>
-      </c>
-    </row>
-    <row r="46" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="31">
-        <v>54002422001</v>
-      </c>
-      <c r="H46" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="I46" s="30">
-        <v>2742</v>
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="2"/>
@@ -8623,30 +8607,26 @@
       <c r="W46"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="50" t="s">
-        <v>632</v>
-      </c>
-      <c r="B47" s="51" t="s">
-        <v>633</v>
-      </c>
-      <c r="C47" s="50" t="s">
-        <v>619</v>
-      </c>
-      <c r="D47" s="50" t="s">
-        <v>634</v>
-      </c>
-      <c r="E47" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="F47" s="50" t="s">
-        <v>635</v>
-      </c>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50">
-        <v>0.3</v>
-      </c>
-      <c r="I47" s="52">
-        <v>3500</v>
+      <c r="A47" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17" t="s">
+        <v>305</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="31">
+        <v>54002422001</v>
+      </c>
+      <c r="H47" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="I47" s="30">
+        <v>2742</v>
       </c>
       <c r="J47" s="51"/>
       <c r="K47" s="51"/>
@@ -8666,9 +8646,35 @@
       <c r="Y47" s="51"/>
       <c r="Z47" s="51"/>
     </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="B48" t="s">
+        <v>624</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D48" t="s">
+        <v>622</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" s="31">
+        <v>54001601001</v>
+      </c>
+      <c r="H48" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I48" s="30">
+        <v>3510</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I46">
-    <sortCondition ref="A2:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
+    <sortCondition ref="A2:A47"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8679,7 +8685,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8698,7 +8704,7 @@
         <v>431</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>503</v>
+        <v>470</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>239</v>
@@ -8711,951 +8717,887 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>317</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="17">
-        <v>54061</v>
+        <v>54001</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="E2" s="18">
-        <v>105612</v>
+        <v>16633</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>318</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="B3" s="4"/>
       <c r="C3" s="17">
-        <v>54039</v>
+        <v>54003</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="20">
-        <v>183279</v>
+        <v>193</v>
+      </c>
+      <c r="E3" s="18">
+        <v>126069</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C4" s="17">
-        <v>54069</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="18">
-        <v>41447</v>
+      <c r="A4" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="58">
+        <v>54005</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="59">
+        <v>21809</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>320</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="17">
-        <v>54037</v>
+        <v>54007</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>7</v>
+        <v>194</v>
       </c>
       <c r="E5" s="18">
-        <v>57146</v>
+        <v>12247</v>
       </c>
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C6" s="17">
-        <v>54055</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="18">
-        <v>58758</v>
+      <c r="A6" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>335</v>
+      </c>
+      <c r="C6" s="58">
+        <v>54009</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="59">
+        <v>21939</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>322</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="17">
-        <v>54041</v>
+        <v>54011</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="18">
-        <v>16166</v>
+        <v>157</v>
+      </c>
+      <c r="E7" s="20">
+        <v>96319</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>323</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="17">
-        <v>54057</v>
+        <v>54013</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="E8" s="18">
-        <v>26868</v>
+        <v>6176</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>324</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="17">
-        <v>54051</v>
+        <v>54015</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>5</v>
+        <v>196</v>
       </c>
       <c r="E9" s="18">
-        <v>30531</v>
+        <v>7892</v>
       </c>
       <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C10" s="17">
-        <v>54065</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="18">
-        <v>17884</v>
+      <c r="A10" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>328</v>
+      </c>
+      <c r="C10" s="58">
+        <v>54017</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="59">
+        <v>8448</v>
       </c>
       <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="C11" s="17">
-        <v>54077</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="18">
-        <v>33432</v>
+      <c r="A11" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11" s="58">
+        <v>54019</v>
+      </c>
+      <c r="D11" s="58" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" s="59">
+        <v>39927</v>
       </c>
       <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>327</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="17">
-        <v>54107</v>
+        <v>54021</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>54</v>
+        <v>198</v>
       </c>
       <c r="E12" s="18">
-        <v>83518</v>
+        <v>7377</v>
       </c>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="C13" s="17">
-        <v>54017</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="18">
-        <v>8448</v>
+      <c r="A13" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58">
+        <v>54023</v>
+      </c>
+      <c r="D13" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="59">
+        <v>11616</v>
       </c>
       <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>329</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="17">
-        <v>54049</v>
+        <v>54025</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>89</v>
+        <v>199</v>
       </c>
       <c r="E14" s="18">
-        <v>56072</v>
+        <v>32608</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="17">
+        <v>54027</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E15" s="18">
+        <v>23302</v>
+      </c>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="58">
+        <v>54029</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="E16" s="59">
+        <v>28656</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="57" t="s">
+        <v>433</v>
+      </c>
+      <c r="C17" s="58">
+        <v>54031</v>
+      </c>
+      <c r="D17" s="58" t="s">
+        <v>202</v>
+      </c>
+      <c r="E17" s="59">
+        <v>14160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B18" s="57" t="s">
         <v>330</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C18" s="58">
         <v>54033</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D18" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E18" s="59">
         <v>67256</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="C16" s="17">
-        <v>54091</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="18">
-        <v>16695</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C17" s="17">
-        <v>54073</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="18">
-        <v>7482</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="C18" s="17">
-        <v>54005</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="18">
-        <v>21809</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>334</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="17">
-        <v>54083</v>
+        <v>54035</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="E19" s="18">
-        <v>28695</v>
+        <v>27738</v>
       </c>
       <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C20" s="17">
-        <v>54009</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="18">
-        <v>21939</v>
+      <c r="A20" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>320</v>
+      </c>
+      <c r="C20" s="58">
+        <v>54037</v>
+      </c>
+      <c r="D20" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="59">
+        <v>57146</v>
       </c>
       <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="C21" s="17">
-        <v>54053</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E21" s="18">
-        <v>26700</v>
+      <c r="A21" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="57" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="58">
+        <v>54039</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="60">
+        <v>183279</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="C22" s="17">
-        <v>54001</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="18">
-        <v>16633</v>
+      <c r="A22" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="C22" s="58">
+        <v>54041</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="59">
+        <v>16166</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>433</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="B23" s="4"/>
       <c r="C23" s="17">
-        <v>54003</v>
+        <v>54043</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="E23" s="18">
-        <v>126069</v>
+        <v>20126</v>
       </c>
       <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>434</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="17">
-        <v>54007</v>
+        <v>54045</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="E24" s="18">
-        <v>12247</v>
+        <v>31909</v>
       </c>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="C25" s="17">
-        <v>54011</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E25" s="20">
-        <v>96319</v>
+      <c r="A25" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="57" t="s">
+        <v>329</v>
+      </c>
+      <c r="C25" s="58">
+        <v>54049</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="59">
+        <v>56072</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="C26" s="17">
-        <v>54013</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="E26" s="18">
-        <v>6176</v>
+      <c r="A26" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="57" t="s">
+        <v>324</v>
+      </c>
+      <c r="C26" s="58">
+        <v>54051</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="59">
+        <v>30531</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="C27" s="17">
-        <v>54015</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="E27" s="18">
-        <v>7892</v>
+      <c r="A27" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="C27" s="58">
+        <v>54053</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" s="59">
+        <v>26700</v>
       </c>
       <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>438</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="B28" s="4"/>
       <c r="C28" s="17">
-        <v>54019</v>
+        <v>54047</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="E28" s="18">
-        <v>39927</v>
+        <v>18363</v>
       </c>
       <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="C29" s="17">
-        <v>54021</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="E29" s="18">
-        <v>7377</v>
+      <c r="A29" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="57" t="s">
+        <v>321</v>
+      </c>
+      <c r="C29" s="58">
+        <v>54055</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="59">
+        <v>58758</v>
       </c>
       <c r="F29" s="22"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="C30" s="17">
-        <v>54023</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E30" s="18">
-        <v>11616</v>
+      <c r="A30" s="57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="57" t="s">
+        <v>323</v>
+      </c>
+      <c r="C30" s="58">
+        <v>54057</v>
+      </c>
+      <c r="D30" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="59">
+        <v>26868</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>441</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="B31" s="4"/>
       <c r="C31" s="17">
-        <v>54025</v>
+        <v>54059</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="E31" s="18">
-        <v>32608</v>
+        <v>23005</v>
       </c>
       <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="C32" s="17">
-        <v>54027</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" s="18">
-        <v>23302</v>
+      <c r="A32" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="57" t="s">
+        <v>317</v>
+      </c>
+      <c r="C32" s="58">
+        <v>54061</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="59">
+        <v>105612</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>443</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B33" s="4"/>
       <c r="C33" s="17">
-        <v>54029</v>
+        <v>54063</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="E33" s="18">
-        <v>28656</v>
+        <v>12332</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="C34" s="17">
-        <v>54031</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E34" s="18">
-        <v>14160</v>
+      <c r="A34" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="57" t="s">
+        <v>325</v>
+      </c>
+      <c r="C34" s="58">
+        <v>54065</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="59">
+        <v>17884</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>445</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B35" s="4"/>
       <c r="C35" s="17">
-        <v>54035</v>
+        <v>54067</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="E35" s="18">
-        <v>27738</v>
+        <v>24300</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C36" s="17">
-        <v>54043</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E36" s="18">
-        <v>20126</v>
+      <c r="A36" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="57" t="s">
+        <v>319</v>
+      </c>
+      <c r="C36" s="58">
+        <v>54069</v>
+      </c>
+      <c r="D36" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="59">
+        <v>41447</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>447</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="B37" s="4"/>
       <c r="C37" s="17">
-        <v>54045</v>
+        <v>54071</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E37" s="18">
-        <v>31909</v>
+        <v>6142</v>
       </c>
       <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C38" s="17">
-        <v>54047</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="E38" s="18">
-        <v>18363</v>
+      <c r="A38" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="57" t="s">
+        <v>332</v>
+      </c>
+      <c r="C38" s="58">
+        <v>54073</v>
+      </c>
+      <c r="D38" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="59">
+        <v>7482</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>449</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="B39" s="4"/>
       <c r="C39" s="17">
-        <v>54059</v>
+        <v>54075</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E39" s="18">
-        <v>23005</v>
+        <v>7841</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>450</v>
-      </c>
-      <c r="C40" s="17">
-        <v>54063</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="E40" s="18">
-        <v>12332</v>
+      <c r="A40" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="57" t="s">
+        <v>326</v>
+      </c>
+      <c r="C40" s="58">
+        <v>54077</v>
+      </c>
+      <c r="D40" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="59">
+        <v>33432</v>
       </c>
       <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>451</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="B41" s="4"/>
       <c r="C41" s="17">
-        <v>54067</v>
+        <v>54079</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="E41" s="18">
-        <v>24300</v>
+        <v>159</v>
+      </c>
+      <c r="E41" s="20">
+        <v>55486</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>452</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="B42" s="4"/>
       <c r="C42" s="17">
-        <v>54071</v>
+        <v>54081</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E42" s="18">
-        <v>6142</v>
+        <v>73771</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>453</v>
-      </c>
-      <c r="C43" s="17">
-        <v>54075</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="E43" s="18">
-        <v>7841</v>
+      <c r="A43" s="57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="57" t="s">
+        <v>334</v>
+      </c>
+      <c r="C43" s="58">
+        <v>54083</v>
+      </c>
+      <c r="D43" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" s="59">
+        <v>28695</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>454</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="B44" s="4"/>
       <c r="C44" s="17">
-        <v>54079</v>
+        <v>54085</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E44" s="20">
-        <v>55486</v>
+        <v>213</v>
+      </c>
+      <c r="E44" s="18">
+        <v>8383</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>455</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="B45" s="4"/>
       <c r="C45" s="17">
-        <v>54081</v>
+        <v>54087</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E45" s="18">
-        <v>73771</v>
+        <v>13898</v>
       </c>
       <c r="F45" s="19"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>213</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>456</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="B46" s="4"/>
       <c r="C46" s="17">
-        <v>54085</v>
+        <v>54089</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E46" s="18">
-        <v>8383</v>
+        <v>11908</v>
       </c>
       <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="C47" s="17">
-        <v>54087</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="E47" s="18">
-        <v>13898</v>
+      <c r="A47" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="57" t="s">
+        <v>331</v>
+      </c>
+      <c r="C47" s="58">
+        <v>54091</v>
+      </c>
+      <c r="D47" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="59">
+        <v>16695</v>
       </c>
       <c r="F47" s="19"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>458</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="B48" s="4"/>
       <c r="C48" s="17">
-        <v>54089</v>
+        <v>54093</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E48" s="18">
-        <v>11908</v>
+        <v>6672</v>
       </c>
       <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="C49" s="17">
-        <v>54093</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="E49" s="18">
-        <v>6672</v>
+      <c r="A49" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B49" s="57"/>
+      <c r="C49" s="58">
+        <v>54095</v>
+      </c>
+      <c r="D49" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" s="59">
+        <v>8811</v>
       </c>
       <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>460</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="B50" s="4"/>
       <c r="C50" s="17">
-        <v>54095</v>
+        <v>54097</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>129</v>
+        <v>217</v>
       </c>
       <c r="E50" s="18">
-        <v>8811</v>
+        <v>23791</v>
       </c>
       <c r="F50" s="19"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>461</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="B51" s="4"/>
       <c r="C51" s="17">
-        <v>54097</v>
+        <v>54099</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="E51" s="18">
-        <v>23791</v>
+        <v>164</v>
+      </c>
+      <c r="E51" s="20">
+        <v>42481</v>
       </c>
       <c r="F51" s="19"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>462</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="B52" s="4"/>
       <c r="C52" s="17">
-        <v>54099</v>
+        <v>54101</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E52" s="20">
-        <v>42481</v>
+        <v>218</v>
+      </c>
+      <c r="E52" s="18">
+        <v>8249</v>
       </c>
       <c r="F52" s="19"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>463</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="B53" s="4"/>
       <c r="C53" s="17">
-        <v>54101</v>
+        <v>54103</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E53" s="18">
-        <v>8249</v>
+        <v>14170</v>
       </c>
       <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>464</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="B54" s="4"/>
       <c r="C54" s="17">
-        <v>54103</v>
+        <v>54105</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E54" s="18">
-        <v>14170</v>
+        <v>5063</v>
       </c>
       <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="C55" s="17">
-        <v>54105</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E55" s="18">
-        <v>5063</v>
+      <c r="A55" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="57" t="s">
+        <v>327</v>
+      </c>
+      <c r="C55" s="58">
+        <v>54107</v>
+      </c>
+      <c r="D55" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="59">
+        <v>83518</v>
       </c>
       <c r="F55" s="19"/>
     </row>
@@ -9663,9 +9605,7 @@
       <c r="A56" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>466</v>
-      </c>
+      <c r="B56" s="4"/>
       <c r="C56" s="17">
         <v>54109</v>
       </c>
@@ -9698,8 +9638,8 @@
       <c r="F62" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:E56">
-    <sortCondition ref="D2:D56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E56">
+    <sortCondition ref="A2:A56"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9709,7 +9649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
@@ -9766,7 +9706,7 @@
     </row>
     <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>585</v>
+        <v>552</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>409</v>
@@ -9786,10 +9726,10 @@
     </row>
     <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>586</v>
+        <v>553</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>601</v>
+        <v>568</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>417</v>
@@ -9818,7 +9758,7 @@
     </row>
     <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>587</v>
+        <v>554</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>399</v>
@@ -9839,7 +9779,7 @@
     </row>
     <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
-        <v>588</v>
+        <v>555</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>400</v>
@@ -9859,10 +9799,10 @@
     </row>
     <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>589</v>
+        <v>556</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>598</v>
+        <v>565</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>416</v>
@@ -9916,10 +9856,10 @@
     </row>
     <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="43" t="s">
-        <v>590</v>
+        <v>557</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>602</v>
+        <v>569</v>
       </c>
       <c r="C11" s="25" t="s">
         <v>417</v>
@@ -9928,12 +9868,12 @@
         <v>382</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>607</v>
+        <v>574</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
-        <v>599</v>
+        <v>566</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>395</v>
@@ -9953,7 +9893,7 @@
     </row>
     <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>600</v>
+        <v>567</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>398</v>
@@ -9974,10 +9914,10 @@
     </row>
     <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>644</v>
+        <v>611</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>651</v>
+        <v>618</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>416</v>
@@ -9994,7 +9934,7 @@
     </row>
     <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
-        <v>641</v>
+        <v>608</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>412</v>
@@ -10014,7 +9954,7 @@
     </row>
     <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
-        <v>591</v>
+        <v>558</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>403</v>
@@ -10034,7 +9974,7 @@
     </row>
     <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
-        <v>592</v>
+        <v>559</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>407</v>
@@ -10055,7 +9995,7 @@
     </row>
     <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>593</v>
+        <v>560</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>391</v>
@@ -10095,10 +10035,10 @@
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
-        <v>594</v>
+        <v>561</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>603</v>
+        <v>570</v>
       </c>
       <c r="C20" s="25" t="s">
         <v>417</v>
@@ -10112,10 +10052,10 @@
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
-        <v>595</v>
+        <v>562</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>606</v>
+        <v>573</v>
       </c>
       <c r="C21" s="25" t="s">
         <v>417</v>
@@ -10129,10 +10069,10 @@
     </row>
     <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
-        <v>596</v>
+        <v>563</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>604</v>
+        <v>571</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>417</v>
@@ -10146,10 +10086,10 @@
     </row>
     <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
-        <v>597</v>
+        <v>564</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>605</v>
+        <v>572</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>417</v>
@@ -10285,23 +10225,23 @@
         <v>374</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>614</v>
+        <v>581</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>586</v>
+        <v>553</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>609</v>
+        <v>576</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>636</v>
+        <v>603</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>612</v>
+        <v>579</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -10317,31 +10257,31 @@
         <v>386</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>637</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>590</v>
+        <v>557</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>608</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>599</v>
+        <v>566</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>610</v>
+        <v>577</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>600</v>
+        <v>567</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -10349,7 +10289,7 @@
         <v>393</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>638</v>
+        <v>605</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -10357,7 +10297,7 @@
         <v>393</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>639</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -10365,12 +10305,12 @@
         <v>393</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>640</v>
+        <v>607</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>593</v>
+        <v>560</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>323</v>
@@ -10378,42 +10318,42 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>641</v>
+        <v>608</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>642</v>
+        <v>609</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
-        <v>592</v>
+        <v>559</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
-        <v>588</v>
+        <v>555</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
-        <v>589</v>
+        <v>556</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>643</v>
+        <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
-        <v>644</v>
+        <v>611</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>611</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10452,10 +10392,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
-        <v>645</v>
+        <v>612</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>646</v>
+        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -10463,7 +10403,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>647</v>
+        <v>614</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -10471,7 +10411,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>648</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -10491,7 +10431,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>649</v>
+        <v>616</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -10499,7 +10439,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>650</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added current date and epiweek to UI.
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370D7818-8CB1-0B49-BB60-62C23B6BA3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8099E5-1D11-C34D-811F-5AEA3BF7A012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="55020" yWindow="4560" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="628">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1924,6 +1924,9 @@
   </si>
   <si>
     <t>L01</t>
+  </si>
+  <si>
+    <t>Host</t>
   </si>
 </sst>
 </file>
@@ -2594,11 +2597,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7378,7 +7381,7 @@
   <dimension ref="A1:Z48"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -9668,9 +9671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10138,6 +10141,23 @@
       </c>
       <c r="F24" s="25" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
+        <v>603</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>627</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>627</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Summersville to site list
</commit_message>
<xml_diff>
--- a/patchr/resources/watchdb.all_tables.xlsx
+++ b/patchr/resources/watchdb.all_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpd0001/github/watch-wv/patchr/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8099E5-1D11-C34D-811F-5AEA3BF7A012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C064E69-35E9-9649-8B94-8E02FDA8AB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55020" yWindow="4560" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="24500" windowHeight="18980" activeTab="1" xr2:uid="{ABEE2980-A2EF-284E-9534-8BF6C1D1D8CC}"/>
   </bookViews>
   <sheets>
     <sheet name="location" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="637">
   <si>
     <t>CharlestonWWTP-01</t>
   </si>
@@ -1845,9 +1845,6 @@
     <t>HometownWWTP</t>
   </si>
   <si>
-    <t xml:space="preserve"> 54079-002-01-00-00</t>
-  </si>
-  <si>
     <t>Putnam PSD</t>
   </si>
   <si>
@@ -1927,6 +1924,36 @@
   </si>
   <si>
     <t>Host</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>W01</t>
+  </si>
+  <si>
+    <t>SummersvilleWWTP-01</t>
+  </si>
+  <si>
+    <t>Summersville</t>
+  </si>
+  <si>
+    <t>SummersvilleWWTP</t>
+  </si>
+  <si>
+    <t>Summersville WWTP</t>
+  </si>
+  <si>
+    <t>Town of Summersville</t>
+  </si>
+  <si>
+    <t>WV0020630</t>
+  </si>
+  <si>
+    <t>54079-002-01-00-00</t>
+  </si>
+  <si>
+    <t>54067-001-01-00-00</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1963,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2094,6 +2121,24 @@
       <color rgb="FF7030A0"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2140,7 +2185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2275,6 +2320,23 @@
     <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2595,13 +2657,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0856F7A-D0C0-3942-9027-9FB2F3C2C3E0}">
-  <dimension ref="A1:T82"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q29" sqref="Q29"/>
+      <selection pane="bottomRight" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3096,7 +3158,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>351</v>
@@ -7314,10 +7376,10 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B82" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>351</v>
@@ -7326,7 +7388,7 @@
         <v>181</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>340</v>
@@ -7341,7 +7403,7 @@
         <v>39.115929999999999</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>202</v>
@@ -7363,6 +7425,65 @@
       </c>
       <c r="S82" s="1">
         <v>26836</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B83" t="s">
+        <v>628</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H83" s="2">
+        <v>-80.910900499999997</v>
+      </c>
+      <c r="I83" s="2">
+        <v>38.301869799999999</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L83" s="28">
+        <v>3791</v>
+      </c>
+      <c r="M83" s="36" t="s">
+        <v>337</v>
+      </c>
+      <c r="N83" s="8">
+        <v>24</v>
+      </c>
+      <c r="O83" s="8">
+        <v>25</v>
+      </c>
+      <c r="P83" s="8">
+        <v>30</v>
+      </c>
+      <c r="Q83" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="R83" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S83" s="1">
+        <v>26651</v>
       </c>
     </row>
   </sheetData>
@@ -7378,10 +7499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7706D3C3-8C4A-6E4A-999A-41BCCB2FAC67}">
-  <dimension ref="A1:Z48"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -7485,134 +7606,134 @@
         <v>2391</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="61" t="s">
         <v>356</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="61"/>
+      <c r="C4" s="61" t="s">
         <v>364</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="61"/>
+      <c r="E4" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="64" t="s">
         <v>540</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="63">
         <v>54000601001</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="61">
         <v>1.8</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="61">
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="61" t="s">
         <v>245</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="61" t="s">
         <v>278</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="61" t="s">
         <v>313</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="64" t="s">
         <v>541</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="63">
         <v>54000101001</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="61">
         <v>0.36499999999999999</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="65">
         <v>1974</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="61" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17" t="s">
+      <c r="B6" s="61"/>
+      <c r="C6" s="61" t="s">
         <v>279</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="61" t="s">
         <v>310</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="64" t="s">
         <v>542</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="63">
         <v>54003031001</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="61">
         <v>0.05</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="61">
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="61" t="s">
         <v>247</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="61" t="s">
         <v>280</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="61" t="s">
         <v>314</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="64" t="s">
         <v>543</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="63">
         <v>54001702001</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="61">
         <v>3</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="65">
         <v>6984</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="61" t="s">
         <v>248</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="61"/>
+      <c r="E8" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="64" t="s">
         <v>544</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="63">
         <v>54002510001</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="61">
         <v>0.21</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="65">
         <v>1340</v>
       </c>
     </row>
@@ -7807,28 +7928,28 @@
         <v>13156</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
+    <row r="16" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="61" t="s">
         <v>254</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="61"/>
+      <c r="C16" s="61" t="s">
         <v>286</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17" t="s">
+      <c r="D16" s="61"/>
+      <c r="E16" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="64" t="s">
         <v>545</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="63">
         <v>54002405001</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="61">
         <v>9</v>
       </c>
-      <c r="I16" s="30">
+      <c r="I16" s="65">
         <v>25525</v>
       </c>
     </row>
@@ -7913,26 +8034,26 @@
         <v>6071</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="61" t="s">
         <v>234</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="61"/>
+      <c r="C20" s="61" t="s">
         <v>290</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="61" t="s">
         <v>236</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="17">
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="61">
         <v>0.5</v>
       </c>
-      <c r="I20" s="30">
+      <c r="I20" s="65">
         <v>1948</v>
       </c>
     </row>
@@ -7941,19 +8062,19 @@
         <v>599</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>600</v>
+        <v>635</v>
       </c>
       <c r="C21" s="49" t="s">
         <v>586</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E21" s="49" t="s">
         <v>159</v>
       </c>
       <c r="F21" s="49" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G21" s="49"/>
       <c r="H21" s="49">
@@ -8179,70 +8300,70 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
+    <row r="30" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="61" t="s">
         <v>354</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="61"/>
+      <c r="C30" s="61" t="s">
         <v>366</v>
       </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17" t="s">
+      <c r="D30" s="61"/>
+      <c r="E30" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17">
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61">
         <v>0.125</v>
       </c>
-      <c r="I30" s="17">
+      <c r="I30" s="61">
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
+    <row r="31" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="61" t="s">
         <v>354</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="61"/>
+      <c r="C31" s="61" t="s">
         <v>366</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="17" t="s">
+      <c r="D31" s="64"/>
+      <c r="E31" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4">
+      <c r="F31" s="61"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="64">
         <v>0.125</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="64">
         <v>1000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
+    <row r="32" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="61" t="s">
         <v>263</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17" t="s">
+      <c r="B32" s="61"/>
+      <c r="C32" s="61" t="s">
         <v>297</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17" t="s">
+      <c r="D32" s="61"/>
+      <c r="E32" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="61" t="s">
         <v>539</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="61">
         <v>54001205001</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H32" s="61">
         <v>1.35</v>
       </c>
-      <c r="I32" s="30">
+      <c r="I32" s="65">
         <v>2700</v>
       </c>
     </row>
@@ -8377,28 +8498,28 @@
         <v>4050</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:26" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="61" t="s">
         <v>267</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17" t="s">
+      <c r="B38" s="61"/>
+      <c r="C38" s="61" t="s">
         <v>300</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17" t="s">
+      <c r="D38" s="61"/>
+      <c r="E38" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="64" t="s">
         <v>548</v>
       </c>
-      <c r="G38" s="31">
+      <c r="G38" s="63">
         <v>54004804001</v>
       </c>
-      <c r="H38" s="17">
+      <c r="H38" s="61">
         <v>0.3</v>
       </c>
-      <c r="I38" s="30">
+      <c r="I38" s="65">
         <v>1800</v>
       </c>
     </row>
@@ -8485,28 +8606,28 @@
         <v>3255</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
+    <row r="42" spans="1:26" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="61" t="s">
         <v>270</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17" t="s">
+      <c r="B42" s="61"/>
+      <c r="C42" s="61" t="s">
         <v>302</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17" t="s">
+      <c r="D42" s="61"/>
+      <c r="E42" s="61" t="s">
         <v>122</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="61" t="s">
         <v>538</v>
       </c>
-      <c r="G42" s="31">
+      <c r="G42" s="63">
         <v>54000509001</v>
       </c>
-      <c r="H42" s="17">
+      <c r="H42" s="61">
         <v>4</v>
       </c>
-      <c r="I42" s="30">
+      <c r="I42" s="65">
         <v>20411</v>
       </c>
     </row>
@@ -8665,33 +8786,62 @@
       <c r="Y47" s="50"/>
       <c r="Z47" s="50"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="17" t="s">
+    <row r="48" spans="1:26" s="62" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="61" t="s">
+        <v>620</v>
+      </c>
+      <c r="B48" s="62" t="s">
+        <v>623</v>
+      </c>
+      <c r="C48" s="62" t="s">
         <v>621</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" s="62" t="s">
+        <v>621</v>
+      </c>
+      <c r="E48" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="F48" s="61" t="s">
         <v>624</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="D48" t="s">
-        <v>622</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>625</v>
-      </c>
-      <c r="G48" s="31">
+      <c r="G48" s="63">
         <v>54001601001</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48" s="64">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I48" s="30">
+      <c r="I48" s="65">
         <v>3510</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="B49" s="66" t="s">
+        <v>636</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>632</v>
+      </c>
+      <c r="D49" t="s">
+        <v>633</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>634</v>
+      </c>
+      <c r="G49" s="31">
+        <v>54003404001</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I49" s="60">
+        <v>3791</v>
       </c>
     </row>
   </sheetData>
@@ -8707,7 +8857,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9284,17 +9434,19 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="57" t="s">
         <v>209</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="17">
+      <c r="B35" s="56" t="s">
+        <v>627</v>
+      </c>
+      <c r="C35" s="57">
         <v>54067</v>
       </c>
-      <c r="D35" s="17" t="s">
+      <c r="D35" s="57" t="s">
         <v>209</v>
       </c>
-      <c r="E35" s="18">
+      <c r="E35" s="58">
         <v>24300</v>
       </c>
     </row>
@@ -9671,7 +9823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C28A9-51BA-1349-BC2C-74CFA9B6CA14}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
@@ -9936,10 +10088,10 @@
     </row>
     <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C14" s="25" t="s">
         <v>416</v>
@@ -9956,7 +10108,7 @@
     </row>
     <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>412</v>
@@ -10145,16 +10297,16 @@
     </row>
     <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E25" s="25" t="s">
         <v>382</v>
@@ -10277,7 +10429,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>579</v>
@@ -10296,7 +10448,7 @@
         <v>386</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -10328,7 +10480,7 @@
         <v>393</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -10336,7 +10488,7 @@
         <v>393</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -10344,7 +10496,7 @@
         <v>393</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -10357,10 +10509,10 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
+        <v>607</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>608</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10368,7 +10520,7 @@
         <v>559</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10376,7 +10528,7 @@
         <v>555</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10384,12 +10536,12 @@
         <v>556</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>578</v>
@@ -10431,10 +10583,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
+        <v>611</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>612</v>
-      </c>
-      <c r="B1" s="54" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -10442,7 +10594,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -10450,7 +10602,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -10470,7 +10622,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -10478,7 +10630,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="55" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>